<commit_message>
Testing versions of models
</commit_message>
<xml_diff>
--- a/Data Info/DadosEscolhidos.xlsx
+++ b/Data Info/DadosEscolhidos.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/ad5e0ae908eb1af8/Documentos/GitHub/gdp-forecasting-with-ML/Data Info/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1671" documentId="11_AD4D361C20488DEA4E38A0E30418638E5BDEDD8E" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{073AE1E5-9F77-45A6-A7E0-7CF50EC135AB}"/>
+  <xr:revisionPtr revIDLastSave="2225" documentId="11_AD4D361C20488DEA4E38A0E30418638E5BDEDD8E" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{58D1A83B-A3FC-4368-8EC0-C5C76B38FE96}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-45" yWindow="-16320" windowWidth="29040" windowHeight="15720" firstSheet="2" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Official Series - Quarterly" sheetId="7" r:id="rId1"/>
@@ -19,7 +19,8 @@
     <sheet name="Table M" sheetId="10" r:id="rId4"/>
     <sheet name="All Series" sheetId="1" state="hidden" r:id="rId5"/>
     <sheet name="All Series (2)" sheetId="6" state="hidden" r:id="rId6"/>
-    <sheet name="exports_SAseries" sheetId="3" r:id="rId7"/>
+    <sheet name="Planilha1" sheetId="11" r:id="rId7"/>
+    <sheet name="exports_SAseries" sheetId="3" state="hidden" r:id="rId8"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Official Series - Quarterly'!$A$1:$J$101</definedName>
@@ -45,7 +46,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6228" uniqueCount="573">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6303" uniqueCount="630">
   <si>
     <t>NSAprod_cam_br</t>
   </si>
@@ -1801,12 +1802,187 @@
   <si>
     <t>Índice de preços IGP-M (1º decêndio e 2º decêndio) - Variação acumulada em 3 meses</t>
   </si>
+  <si>
+    <t>lasso_model1q</t>
+  </si>
+  <si>
+    <t>benchmark1q</t>
+  </si>
+  <si>
+    <t>enet_model1q</t>
+  </si>
+  <si>
+    <t xml:space="preserve"># h=1 </t>
+  </si>
+  <si>
+    <t xml:space="preserve"># h=4 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">RMSE </t>
+  </si>
+  <si>
+    <t>MAE</t>
+  </si>
+  <si>
+    <t>MAPE</t>
+  </si>
+  <si>
+    <t>benchmark2q</t>
+  </si>
+  <si>
+    <t>lasso_model2q</t>
+  </si>
+  <si>
+    <t>enet_model2q</t>
+  </si>
+  <si>
+    <t>benchmark3q</t>
+  </si>
+  <si>
+    <t>lasso_model3q</t>
+  </si>
+  <si>
+    <t>enet_model3q</t>
+  </si>
+  <si>
+    <t>benchmark4q</t>
+  </si>
+  <si>
+    <t>lasso_model4q</t>
+  </si>
+  <si>
+    <t>enet_model4q</t>
+  </si>
+  <si>
+    <t>benchmark5q</t>
+  </si>
+  <si>
+    <t>lasso_model5q</t>
+  </si>
+  <si>
+    <t>enet_model5q</t>
+  </si>
+  <si>
+    <t>- raw_gdp made by mean, no logs, no dummies</t>
+  </si>
+  <si>
+    <t>- raw_gdp made by mean, no logs, all dummies</t>
+  </si>
+  <si>
+    <t>- raw_gdp made by mean, no logs, no dflood</t>
+  </si>
+  <si>
+    <t>- raw_gdp made by mean, no logs, no dshift</t>
+  </si>
+  <si>
+    <t>- raw_gdp made by mean, no logs, only dpandemic</t>
+  </si>
+  <si>
+    <t>1st try - logmresults ----------- old log fun</t>
+  </si>
+  <si>
+    <t>2nd try - logwresults ----------- new log fun</t>
+  </si>
+  <si>
+    <t>3rd try - rawm_ibc ----------- no log, raw data</t>
+  </si>
+  <si>
+    <t>4th try - rawm_stry --------- no log fun, but adf test</t>
+  </si>
+  <si>
+    <t>benchmark1w</t>
+  </si>
+  <si>
+    <t>lasso_model1w</t>
+  </si>
+  <si>
+    <t>enet_model1w</t>
+  </si>
+  <si>
+    <t>benchmark2w</t>
+  </si>
+  <si>
+    <t>lasso_model2w</t>
+  </si>
+  <si>
+    <t>enet_model2w</t>
+  </si>
+  <si>
+    <t>benchmark3w</t>
+  </si>
+  <si>
+    <t>lasso_model3w</t>
+  </si>
+  <si>
+    <t>enet_model3w</t>
+  </si>
+  <si>
+    <t>benchmark4w</t>
+  </si>
+  <si>
+    <t>lasso_model4w</t>
+  </si>
+  <si>
+    <t>enet_model4w</t>
+  </si>
+  <si>
+    <t># h=12</t>
+  </si>
+  <si>
+    <t>6 monthly, 6 quarterly</t>
+  </si>
+  <si>
+    <t>title h = 1</t>
+  </si>
+  <si>
+    <t>title h=12</t>
+  </si>
+  <si>
+    <t>half legend</t>
+  </si>
+  <si>
+    <t>other half, no leg title</t>
+  </si>
+  <si>
+    <t>lasso</t>
+  </si>
+  <si>
+    <t>enet</t>
+  </si>
+  <si>
+    <t>rf</t>
+  </si>
+  <si>
+    <t>benchmark</t>
+  </si>
+  <si>
+    <t>lasso_model</t>
+  </si>
+  <si>
+    <t>enet_model</t>
+  </si>
+  <si>
+    <t>rf_model</t>
+  </si>
+  <si>
+    <t>rf_model2w</t>
+  </si>
+  <si>
+    <t>datasetm</t>
+  </si>
+  <si>
+    <t>old log, seas nsdiffs</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="7" x14ac:knownFonts="1">
+  <numFmts count="2">
+    <numFmt numFmtId="170" formatCode="#,##0.0000"/>
+    <numFmt numFmtId="181" formatCode="0.0000"/>
+  </numFmts>
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1854,8 +2030,20 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="7"/>
+      <color rgb="FF4D4D4C"/>
+      <name val="Cascadia Code"/>
+      <family val="3"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="5">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1880,12 +2068,33 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF92D050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
       <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
       <bottom/>
       <diagonal/>
     </border>
@@ -1895,7 +2104,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="25">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -1914,6 +2123,43 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="4" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="170" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="170" fontId="7" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="4" fontId="7" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="4" fontId="7" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="4" fontId="7" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="170" fontId="7" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="170" fontId="7" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="170" fontId="7" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="170" fontId="7" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="181" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -2204,8 +2450,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5BC43247-4F7A-412E-B82F-0C6D32656462}">
   <dimension ref="A1:P155"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="C1" sqref="C1:I1048576"/>
+    <sheetView topLeftCell="A61" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="H101" sqref="H101"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2288,7 +2534,7 @@
         <v>227</v>
       </c>
       <c r="N2">
-        <f t="shared" ref="N2:N16" si="0">COUNTIFS(I:I,M2)</f>
+        <f t="shared" ref="N2:N7" si="0">COUNTIFS(I:I,M2)</f>
         <v>8</v>
       </c>
       <c r="O2">
@@ -2554,7 +2800,7 @@
         <v>224</v>
       </c>
       <c r="N8">
-        <f>COUNTIFS(I:I,M8)</f>
+        <f t="shared" ref="N8:N14" si="1">COUNTIFS(I:I,M8)</f>
         <v>6</v>
       </c>
     </row>
@@ -2596,7 +2842,7 @@
         <v>238</v>
       </c>
       <c r="N9">
-        <f>COUNTIFS(I:I,M9)</f>
+        <f t="shared" si="1"/>
         <v>6</v>
       </c>
     </row>
@@ -2638,7 +2884,7 @@
         <v>233</v>
       </c>
       <c r="N10">
-        <f>COUNTIFS(I:I,M10)</f>
+        <f t="shared" si="1"/>
         <v>7</v>
       </c>
     </row>
@@ -2680,7 +2926,7 @@
         <v>225</v>
       </c>
       <c r="N11">
-        <f>COUNTIFS(I:I,M11)</f>
+        <f t="shared" si="1"/>
         <v>3</v>
       </c>
     </row>
@@ -2722,7 +2968,7 @@
         <v>230</v>
       </c>
       <c r="N12">
-        <f>COUNTIFS(I:I,M12)</f>
+        <f t="shared" si="1"/>
         <v>6</v>
       </c>
     </row>
@@ -2764,7 +3010,7 @@
         <v>232</v>
       </c>
       <c r="N13">
-        <f>COUNTIFS(I:I,M13)</f>
+        <f t="shared" si="1"/>
         <v>3</v>
       </c>
     </row>
@@ -2806,7 +3052,7 @@
         <v>231</v>
       </c>
       <c r="N14">
-        <f>COUNTIFS(I:I,M14)</f>
+        <f t="shared" si="1"/>
         <v>11</v>
       </c>
     </row>
@@ -3037,7 +3283,7 @@
         <v>545</v>
       </c>
       <c r="N20">
-        <f t="shared" ref="N20" si="1">COUNTIFS(K:K,M20)</f>
+        <f t="shared" ref="N20" si="2">COUNTIFS(K:K,M20)</f>
         <v>7</v>
       </c>
     </row>
@@ -5887,7 +6133,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{07748F0C-CE3F-42B1-961E-411301A80C4F}">
   <dimension ref="A1:P101"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="I19" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView topLeftCell="I19" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="J28" sqref="J28"/>
     </sheetView>
   </sheetViews>
@@ -23320,6 +23566,911 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3870FAA5-0C9A-4077-820D-651F982FFC52}">
+  <dimension ref="H3:Y41"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="D13" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="Q25" sqref="Q25"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="11" max="11" width="8.81640625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="9.54296875" bestFit="1" customWidth="1"/>
+    <col min="13" max="16" width="8.81640625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="3" spans="8:22" x14ac:dyDescent="0.35">
+      <c r="K3" t="s">
+        <v>576</v>
+      </c>
+      <c r="L3" t="s">
+        <v>577</v>
+      </c>
+      <c r="M3" t="s">
+        <v>576</v>
+      </c>
+      <c r="N3" t="s">
+        <v>577</v>
+      </c>
+      <c r="O3" t="s">
+        <v>576</v>
+      </c>
+      <c r="P3" t="s">
+        <v>577</v>
+      </c>
+    </row>
+    <row r="4" spans="8:22" x14ac:dyDescent="0.35">
+      <c r="K4" t="s">
+        <v>578</v>
+      </c>
+      <c r="L4" t="s">
+        <v>578</v>
+      </c>
+      <c r="M4" t="s">
+        <v>579</v>
+      </c>
+      <c r="N4" t="s">
+        <v>579</v>
+      </c>
+      <c r="O4" t="s">
+        <v>580</v>
+      </c>
+      <c r="P4" t="s">
+        <v>580</v>
+      </c>
+    </row>
+    <row r="5" spans="8:22" x14ac:dyDescent="0.35">
+      <c r="I5" s="10" t="s">
+        <v>574</v>
+      </c>
+      <c r="J5" s="10"/>
+      <c r="K5" s="15">
+        <v>10.138339999999999</v>
+      </c>
+      <c r="L5" s="15">
+        <v>11.06123</v>
+      </c>
+      <c r="M5" s="15">
+        <v>7.387079</v>
+      </c>
+      <c r="N5" s="15">
+        <v>7.043361</v>
+      </c>
+      <c r="O5" s="15">
+        <v>5.4638929999999997</v>
+      </c>
+      <c r="P5" s="15">
+        <v>5.0934699999999999</v>
+      </c>
+      <c r="Q5" t="s">
+        <v>593</v>
+      </c>
+    </row>
+    <row r="6" spans="8:22" x14ac:dyDescent="0.35">
+      <c r="I6" s="11" t="s">
+        <v>573</v>
+      </c>
+      <c r="J6" s="11"/>
+      <c r="K6" s="16">
+        <v>5.3373280000000003</v>
+      </c>
+      <c r="L6" s="12">
+        <v>8.0436940000000003</v>
+      </c>
+      <c r="M6" s="12">
+        <v>4.3954370000000003</v>
+      </c>
+      <c r="N6" s="12">
+        <v>6.2554879999999997</v>
+      </c>
+      <c r="O6" s="12">
+        <v>3.273847</v>
+      </c>
+      <c r="P6" s="12">
+        <v>4.6032760000000001</v>
+      </c>
+    </row>
+    <row r="7" spans="8:22" x14ac:dyDescent="0.35">
+      <c r="I7" s="11" t="s">
+        <v>575</v>
+      </c>
+      <c r="J7" s="11"/>
+      <c r="K7" s="17">
+        <v>5.5069629999999998</v>
+      </c>
+      <c r="L7" s="12">
+        <v>7.9476279999999999</v>
+      </c>
+      <c r="M7" s="17">
+        <v>4.2647430000000002</v>
+      </c>
+      <c r="N7" s="12">
+        <v>6.2991429999999999</v>
+      </c>
+      <c r="O7" s="17">
+        <v>3.1697690000000001</v>
+      </c>
+      <c r="P7" s="12">
+        <v>4.6444510000000001</v>
+      </c>
+    </row>
+    <row r="8" spans="8:22" x14ac:dyDescent="0.35">
+      <c r="I8" s="10" t="s">
+        <v>581</v>
+      </c>
+      <c r="J8" s="10"/>
+      <c r="K8" s="15">
+        <v>10.138339999999999</v>
+      </c>
+      <c r="L8" s="15">
+        <v>11.06123</v>
+      </c>
+      <c r="M8" s="15">
+        <v>7.387079</v>
+      </c>
+      <c r="N8" s="15">
+        <v>7.043361</v>
+      </c>
+      <c r="O8" s="15">
+        <v>5.4638929999999997</v>
+      </c>
+      <c r="P8" s="15">
+        <v>5.0934699999999999</v>
+      </c>
+      <c r="Q8" t="s">
+        <v>594</v>
+      </c>
+    </row>
+    <row r="9" spans="8:22" x14ac:dyDescent="0.35">
+      <c r="I9" s="11" t="s">
+        <v>582</v>
+      </c>
+      <c r="J9" s="11"/>
+      <c r="K9" s="12">
+        <v>5.3612840000000004</v>
+      </c>
+      <c r="L9" s="12">
+        <v>7.6462380000000003</v>
+      </c>
+      <c r="M9" s="16">
+        <v>4.273517</v>
+      </c>
+      <c r="N9" s="12">
+        <v>5.8681039999999998</v>
+      </c>
+      <c r="O9" s="16">
+        <v>3.1899090000000001</v>
+      </c>
+      <c r="P9" s="12">
+        <v>4.3203310000000004</v>
+      </c>
+    </row>
+    <row r="10" spans="8:22" x14ac:dyDescent="0.35">
+      <c r="I10" s="11" t="s">
+        <v>583</v>
+      </c>
+      <c r="J10" s="11"/>
+      <c r="K10" s="12">
+        <v>5.9704059999999997</v>
+      </c>
+      <c r="L10" s="17">
+        <v>7.6325320000000003</v>
+      </c>
+      <c r="M10" s="12">
+        <v>4.5451629999999996</v>
+      </c>
+      <c r="N10" s="17">
+        <v>5.8982469999999996</v>
+      </c>
+      <c r="O10" s="12">
+        <v>3.3889990000000001</v>
+      </c>
+      <c r="P10" s="17">
+        <v>4.3434660000000003</v>
+      </c>
+    </row>
+    <row r="11" spans="8:22" x14ac:dyDescent="0.35">
+      <c r="H11" s="18"/>
+      <c r="I11" s="10" t="s">
+        <v>584</v>
+      </c>
+      <c r="J11" s="10"/>
+      <c r="K11" s="15">
+        <v>10.138339999999999</v>
+      </c>
+      <c r="L11" s="15">
+        <v>11.06123</v>
+      </c>
+      <c r="M11" s="15">
+        <v>7.387079</v>
+      </c>
+      <c r="N11" s="15">
+        <v>7.043361</v>
+      </c>
+      <c r="O11" s="15">
+        <v>5.4638929999999997</v>
+      </c>
+      <c r="P11" s="15">
+        <v>5.0934699999999999</v>
+      </c>
+      <c r="Q11" t="s">
+        <v>595</v>
+      </c>
+      <c r="V11" s="18"/>
+    </row>
+    <row r="12" spans="8:22" x14ac:dyDescent="0.35">
+      <c r="H12" s="18"/>
+      <c r="I12" s="11" t="s">
+        <v>585</v>
+      </c>
+      <c r="J12" s="11"/>
+      <c r="K12" s="12">
+        <v>5.3612840000000004</v>
+      </c>
+      <c r="L12" s="12">
+        <v>7.6462380000000003</v>
+      </c>
+      <c r="M12" s="16">
+        <v>4.273517</v>
+      </c>
+      <c r="N12" s="12">
+        <v>5.8681039999999998</v>
+      </c>
+      <c r="O12" s="16">
+        <v>3.1899090000000001</v>
+      </c>
+      <c r="P12" s="12">
+        <v>4.3203310000000004</v>
+      </c>
+      <c r="V12" s="18"/>
+    </row>
+    <row r="13" spans="8:22" x14ac:dyDescent="0.35">
+      <c r="H13" s="18"/>
+      <c r="I13" t="s">
+        <v>586</v>
+      </c>
+      <c r="K13" s="12">
+        <v>5.9704059999999997</v>
+      </c>
+      <c r="L13" s="17">
+        <v>7.6325320000000003</v>
+      </c>
+      <c r="M13" s="12">
+        <v>4.5451629999999996</v>
+      </c>
+      <c r="N13" s="17">
+        <v>5.8982469999999996</v>
+      </c>
+      <c r="O13" s="12">
+        <v>3.3889990000000001</v>
+      </c>
+      <c r="P13" s="17">
+        <v>4.3434660000000003</v>
+      </c>
+      <c r="V13" s="18"/>
+    </row>
+    <row r="14" spans="8:22" x14ac:dyDescent="0.35">
+      <c r="I14" s="10" t="s">
+        <v>587</v>
+      </c>
+      <c r="J14" s="10"/>
+      <c r="K14" s="15">
+        <v>10.138339999999999</v>
+      </c>
+      <c r="L14" s="15">
+        <v>11.06123</v>
+      </c>
+      <c r="M14" s="15">
+        <v>7.387079</v>
+      </c>
+      <c r="N14" s="15">
+        <v>7.043361</v>
+      </c>
+      <c r="O14" s="15">
+        <v>5.4638929999999997</v>
+      </c>
+      <c r="P14" s="15">
+        <v>5.0934699999999999</v>
+      </c>
+      <c r="Q14" t="s">
+        <v>596</v>
+      </c>
+    </row>
+    <row r="15" spans="8:22" x14ac:dyDescent="0.35">
+      <c r="I15" t="s">
+        <v>588</v>
+      </c>
+      <c r="K15" s="12">
+        <v>5.4057740000000001</v>
+      </c>
+      <c r="L15" s="16">
+        <v>7.6163400000000001</v>
+      </c>
+      <c r="M15" s="12">
+        <v>4.3369090000000003</v>
+      </c>
+      <c r="N15" s="16">
+        <v>5.8291069999999996</v>
+      </c>
+      <c r="O15" s="12">
+        <v>3.2369050000000001</v>
+      </c>
+      <c r="P15" s="16">
+        <v>4.291474</v>
+      </c>
+    </row>
+    <row r="16" spans="8:22" x14ac:dyDescent="0.35">
+      <c r="I16" t="s">
+        <v>589</v>
+      </c>
+      <c r="K16" s="12">
+        <v>5.9582610000000003</v>
+      </c>
+      <c r="L16" s="12">
+        <v>7.656339</v>
+      </c>
+      <c r="M16" s="12">
+        <v>4.5040079999999998</v>
+      </c>
+      <c r="N16" s="12">
+        <v>5.9440749999999998</v>
+      </c>
+      <c r="O16" s="12">
+        <v>3.3588460000000002</v>
+      </c>
+      <c r="P16" s="12">
+        <v>4.3810200000000004</v>
+      </c>
+    </row>
+    <row r="17" spans="8:25" x14ac:dyDescent="0.35">
+      <c r="I17" s="10" t="s">
+        <v>590</v>
+      </c>
+      <c r="J17" s="10"/>
+      <c r="K17" s="15">
+        <v>10.138339999999999</v>
+      </c>
+      <c r="L17" s="15">
+        <v>11.06123</v>
+      </c>
+      <c r="M17" s="15">
+        <v>7.387079</v>
+      </c>
+      <c r="N17" s="15">
+        <v>7.043361</v>
+      </c>
+      <c r="O17" s="15">
+        <v>5.4638929999999997</v>
+      </c>
+      <c r="P17" s="15">
+        <v>5.0934699999999999</v>
+      </c>
+      <c r="Q17" t="s">
+        <v>597</v>
+      </c>
+    </row>
+    <row r="18" spans="8:25" x14ac:dyDescent="0.35">
+      <c r="I18" t="s">
+        <v>591</v>
+      </c>
+      <c r="K18" s="12">
+        <v>5.4057740000000001</v>
+      </c>
+      <c r="L18" s="16">
+        <v>7.6163400000000001</v>
+      </c>
+      <c r="M18" s="12">
+        <v>4.3369090000000003</v>
+      </c>
+      <c r="N18" s="16">
+        <v>5.8291069999999996</v>
+      </c>
+      <c r="O18" s="12">
+        <v>3.2369050000000001</v>
+      </c>
+      <c r="P18" s="16">
+        <v>4.291474</v>
+      </c>
+    </row>
+    <row r="19" spans="8:25" x14ac:dyDescent="0.35">
+      <c r="I19" t="s">
+        <v>592</v>
+      </c>
+      <c r="K19" s="12">
+        <v>5.9582610000000003</v>
+      </c>
+      <c r="L19" s="12">
+        <v>7.656339</v>
+      </c>
+      <c r="M19" s="12">
+        <v>4.5040079999999998</v>
+      </c>
+      <c r="N19" s="12">
+        <v>5.9440749999999998</v>
+      </c>
+      <c r="O19" s="12">
+        <v>3.3588460000000002</v>
+      </c>
+      <c r="P19" s="12">
+        <v>4.3810200000000004</v>
+      </c>
+    </row>
+    <row r="22" spans="8:25" x14ac:dyDescent="0.35">
+      <c r="K22" t="s">
+        <v>576</v>
+      </c>
+      <c r="L22" t="s">
+        <v>614</v>
+      </c>
+      <c r="M22" t="s">
+        <v>576</v>
+      </c>
+      <c r="N22" t="s">
+        <v>614</v>
+      </c>
+      <c r="O22" t="s">
+        <v>576</v>
+      </c>
+      <c r="P22" t="s">
+        <v>614</v>
+      </c>
+      <c r="X22" t="s">
+        <v>615</v>
+      </c>
+    </row>
+    <row r="23" spans="8:25" x14ac:dyDescent="0.35">
+      <c r="K23" t="s">
+        <v>578</v>
+      </c>
+      <c r="L23" t="s">
+        <v>578</v>
+      </c>
+      <c r="M23" t="s">
+        <v>579</v>
+      </c>
+      <c r="N23" t="s">
+        <v>579</v>
+      </c>
+      <c r="O23" t="s">
+        <v>580</v>
+      </c>
+      <c r="P23" t="s">
+        <v>580</v>
+      </c>
+    </row>
+    <row r="24" spans="8:25" x14ac:dyDescent="0.35">
+      <c r="I24" t="s">
+        <v>623</v>
+      </c>
+      <c r="K24" s="19">
+        <v>6.6295580000000007E-2</v>
+      </c>
+      <c r="L24" s="13">
+        <v>9.8374290000000003E-2</v>
+      </c>
+      <c r="M24" s="19">
+        <v>4.8804380000000001E-2</v>
+      </c>
+      <c r="N24" s="13">
+        <v>7.0079680000000005E-2</v>
+      </c>
+      <c r="O24" s="19">
+        <v>1.048171</v>
+      </c>
+      <c r="P24" s="13">
+        <v>1.5017780000000001</v>
+      </c>
+      <c r="Q24" t="s">
+        <v>628</v>
+      </c>
+      <c r="R24" t="s">
+        <v>629</v>
+      </c>
+    </row>
+    <row r="25" spans="8:25" x14ac:dyDescent="0.35">
+      <c r="I25" t="s">
+        <v>624</v>
+      </c>
+      <c r="K25" s="13">
+        <v>3.6495979999999997E-2</v>
+      </c>
+      <c r="L25" s="13">
+        <v>5.9897640000000002E-2</v>
+      </c>
+      <c r="M25" s="13">
+        <v>2.8393020000000001E-2</v>
+      </c>
+      <c r="N25" s="13">
+        <v>4.3121090000000001E-2</v>
+      </c>
+      <c r="O25" s="13">
+        <v>0.61500900000000003</v>
+      </c>
+      <c r="P25" s="13">
+        <v>0.93870880000000001</v>
+      </c>
+    </row>
+    <row r="26" spans="8:25" x14ac:dyDescent="0.35">
+      <c r="I26" t="s">
+        <v>625</v>
+      </c>
+      <c r="K26" s="13">
+        <v>5.0724129999999999E-2</v>
+      </c>
+      <c r="L26" s="13">
+        <v>6.4122650000000003E-2</v>
+      </c>
+      <c r="M26" s="13">
+        <v>3.893112E-2</v>
+      </c>
+      <c r="N26" s="13">
+        <v>5.13068E-2</v>
+      </c>
+      <c r="O26" s="13">
+        <v>0.83906159999999996</v>
+      </c>
+      <c r="P26" s="13">
+        <v>1.1120433000000001</v>
+      </c>
+      <c r="X26" t="s">
+        <v>616</v>
+      </c>
+      <c r="Y26" t="s">
+        <v>617</v>
+      </c>
+    </row>
+    <row r="27" spans="8:25" x14ac:dyDescent="0.35">
+      <c r="I27" t="s">
+        <v>626</v>
+      </c>
+      <c r="K27" s="24">
+        <v>5.0135369999999999E-2</v>
+      </c>
+      <c r="L27" s="24">
+        <v>5.4280870000000002E-2</v>
+      </c>
+      <c r="M27" s="24">
+        <v>3.5086409999999998E-2</v>
+      </c>
+      <c r="N27" s="24">
+        <v>4.0220220000000001E-2</v>
+      </c>
+      <c r="O27" s="24">
+        <v>0.75690360000000001</v>
+      </c>
+      <c r="P27" s="24">
+        <v>0.86743199999999998</v>
+      </c>
+      <c r="X27" s="18" t="s">
+        <v>620</v>
+      </c>
+      <c r="Y27" s="18"/>
+    </row>
+    <row r="28" spans="8:25" x14ac:dyDescent="0.35">
+      <c r="H28" s="23"/>
+      <c r="I28" s="10" t="s">
+        <v>602</v>
+      </c>
+      <c r="J28" s="10"/>
+      <c r="K28" s="14">
+        <v>6.7389569999999996E-2</v>
+      </c>
+      <c r="L28" s="20">
+        <v>9.6357360000000003E-2</v>
+      </c>
+      <c r="M28" s="14">
+        <v>5.007342E-2</v>
+      </c>
+      <c r="N28" s="20">
+        <v>6.8928249999999996E-2</v>
+      </c>
+      <c r="O28" s="14">
+        <v>1.0766389999999999</v>
+      </c>
+      <c r="P28" s="20">
+        <v>1.4784839999999999</v>
+      </c>
+      <c r="Q28" t="s">
+        <v>598</v>
+      </c>
+      <c r="U28" s="23"/>
+      <c r="X28" s="18" t="s">
+        <v>621</v>
+      </c>
+      <c r="Y28" s="18"/>
+    </row>
+    <row r="29" spans="8:25" x14ac:dyDescent="0.35">
+      <c r="H29" s="23"/>
+      <c r="I29" t="s">
+        <v>603</v>
+      </c>
+      <c r="K29" s="21">
+        <v>3.5456799999999997E-2</v>
+      </c>
+      <c r="L29" s="21">
+        <v>5.7688940000000001E-2</v>
+      </c>
+      <c r="M29" s="21">
+        <v>2.732362E-2</v>
+      </c>
+      <c r="N29" s="21">
+        <v>4.1704409999999997E-2</v>
+      </c>
+      <c r="O29" s="21">
+        <v>0.59215430000000002</v>
+      </c>
+      <c r="P29" s="21">
+        <v>0.90730739999999999</v>
+      </c>
+      <c r="U29" s="23"/>
+      <c r="X29" s="18" t="s">
+        <v>622</v>
+      </c>
+      <c r="Y29" s="18"/>
+    </row>
+    <row r="30" spans="8:25" x14ac:dyDescent="0.35">
+      <c r="H30" s="23"/>
+      <c r="I30" t="s">
+        <v>604</v>
+      </c>
+      <c r="K30" s="22">
+        <v>4.9312519999999999E-2</v>
+      </c>
+      <c r="L30" s="22">
+        <v>6.2136660000000003E-2</v>
+      </c>
+      <c r="M30" s="22">
+        <v>3.7580210000000003E-2</v>
+      </c>
+      <c r="N30" s="22">
+        <v>4.9575040000000001E-2</v>
+      </c>
+      <c r="O30" s="22">
+        <v>0.81035729999999995</v>
+      </c>
+      <c r="P30" s="22">
+        <v>1.0750708</v>
+      </c>
+      <c r="U30" s="23"/>
+      <c r="X30" t="s">
+        <v>618</v>
+      </c>
+      <c r="Y30" t="s">
+        <v>619</v>
+      </c>
+    </row>
+    <row r="31" spans="8:25" x14ac:dyDescent="0.35">
+      <c r="I31" s="10" t="s">
+        <v>605</v>
+      </c>
+      <c r="J31" s="10"/>
+      <c r="K31" s="14">
+        <v>6.7389569999999996E-2</v>
+      </c>
+      <c r="L31" s="20">
+        <v>9.6357360000000003E-2</v>
+      </c>
+      <c r="M31" s="14">
+        <v>5.007342E-2</v>
+      </c>
+      <c r="N31" s="20">
+        <v>6.8928249999999996E-2</v>
+      </c>
+      <c r="O31" s="14">
+        <v>1.0766389999999999</v>
+      </c>
+      <c r="P31" s="20">
+        <v>1.4784839999999999</v>
+      </c>
+      <c r="Q31" t="s">
+        <v>599</v>
+      </c>
+    </row>
+    <row r="32" spans="8:25" x14ac:dyDescent="0.35">
+      <c r="I32" t="s">
+        <v>606</v>
+      </c>
+      <c r="K32" s="13">
+        <v>0.10952291</v>
+      </c>
+      <c r="L32" s="13">
+        <v>6.3788289999999997E-2</v>
+      </c>
+      <c r="M32" s="13">
+        <v>4.4270120000000003E-2</v>
+      </c>
+      <c r="N32" s="13">
+        <v>4.4905760000000003E-2</v>
+      </c>
+      <c r="O32" s="13">
+        <v>0.96270840000000002</v>
+      </c>
+      <c r="P32" s="13">
+        <v>0.97586759999999995</v>
+      </c>
+    </row>
+    <row r="33" spans="9:17" x14ac:dyDescent="0.35">
+      <c r="I33" t="s">
+        <v>607</v>
+      </c>
+      <c r="K33" s="13">
+        <v>5.2181999999999999E-2</v>
+      </c>
+      <c r="L33" s="13">
+        <v>6.6322430000000002E-2</v>
+      </c>
+      <c r="M33" s="13">
+        <v>3.865532E-2</v>
+      </c>
+      <c r="N33" s="13">
+        <v>5.1502010000000001E-2</v>
+      </c>
+      <c r="O33" s="13">
+        <v>0.83366150000000006</v>
+      </c>
+      <c r="P33" s="13">
+        <v>1.1166924</v>
+      </c>
+    </row>
+    <row r="34" spans="9:17" x14ac:dyDescent="0.35">
+      <c r="I34" t="s">
+        <v>627</v>
+      </c>
+    </row>
+    <row r="36" spans="9:17" x14ac:dyDescent="0.35">
+      <c r="I36" s="10" t="s">
+        <v>608</v>
+      </c>
+      <c r="J36" s="10"/>
+      <c r="K36" s="14">
+        <v>7.3945249999999998</v>
+      </c>
+      <c r="L36" s="14">
+        <v>10.177414000000001</v>
+      </c>
+      <c r="M36" s="14">
+        <v>5.3058959999999997</v>
+      </c>
+      <c r="N36" s="14">
+        <v>7.203055</v>
+      </c>
+      <c r="O36" s="14">
+        <v>5.0400410000000004</v>
+      </c>
+      <c r="P36" s="14">
+        <v>6.8124219999999998</v>
+      </c>
+      <c r="Q36" t="s">
+        <v>600</v>
+      </c>
+    </row>
+    <row r="37" spans="9:17" x14ac:dyDescent="0.35">
+      <c r="I37" t="s">
+        <v>609</v>
+      </c>
+      <c r="K37" s="13">
+        <v>3.7484489999999999</v>
+      </c>
+      <c r="L37" s="13">
+        <v>5.9246020000000001</v>
+      </c>
+      <c r="M37" s="13">
+        <v>2.8394059999999999</v>
+      </c>
+      <c r="N37" s="13">
+        <v>4.3051529999999998</v>
+      </c>
+      <c r="O37" s="13">
+        <v>2.7975469999999998</v>
+      </c>
+      <c r="P37" s="13">
+        <v>4.2833860000000001</v>
+      </c>
+    </row>
+    <row r="38" spans="9:17" x14ac:dyDescent="0.35">
+      <c r="I38" t="s">
+        <v>610</v>
+      </c>
+      <c r="K38" s="13">
+        <v>3.7453059999999998</v>
+      </c>
+      <c r="L38" s="13">
+        <v>5.4190430000000003</v>
+      </c>
+      <c r="M38" s="13">
+        <v>2.8651089999999999</v>
+      </c>
+      <c r="N38" s="13">
+        <v>3.8482769999999999</v>
+      </c>
+      <c r="O38" s="13">
+        <v>2.8197679999999998</v>
+      </c>
+      <c r="P38" s="13">
+        <v>3.8382869999999998</v>
+      </c>
+    </row>
+    <row r="39" spans="9:17" x14ac:dyDescent="0.35">
+      <c r="I39" s="10" t="s">
+        <v>611</v>
+      </c>
+      <c r="J39" s="10"/>
+      <c r="K39" s="14">
+        <v>7.3865740000000004</v>
+      </c>
+      <c r="L39" s="14">
+        <v>10.201127</v>
+      </c>
+      <c r="M39" s="14">
+        <v>5.272157</v>
+      </c>
+      <c r="N39" s="14">
+        <v>7.1923769999999996</v>
+      </c>
+      <c r="O39" s="14">
+        <v>4.9960110000000002</v>
+      </c>
+      <c r="P39" s="14">
+        <v>6.7898480000000001</v>
+      </c>
+      <c r="Q39" t="s">
+        <v>601</v>
+      </c>
+    </row>
+    <row r="40" spans="9:17" x14ac:dyDescent="0.35">
+      <c r="I40" t="s">
+        <v>612</v>
+      </c>
+      <c r="K40" s="13">
+        <v>3.8589190000000002</v>
+      </c>
+      <c r="L40" s="13">
+        <v>5.7759210000000003</v>
+      </c>
+      <c r="M40" s="13">
+        <v>2.9577749999999998</v>
+      </c>
+      <c r="N40" s="13">
+        <v>4.1816709999999997</v>
+      </c>
+      <c r="O40" s="13">
+        <v>2.9247450000000002</v>
+      </c>
+      <c r="P40" s="13">
+        <v>4.1689720000000001</v>
+      </c>
+    </row>
+    <row r="41" spans="9:17" x14ac:dyDescent="0.35">
+      <c r="I41" t="s">
+        <v>613</v>
+      </c>
+      <c r="K41" s="13">
+        <v>3.8382070000000001</v>
+      </c>
+      <c r="L41" s="13">
+        <v>5.5115879999999997</v>
+      </c>
+      <c r="M41" s="13">
+        <v>2.981779</v>
+      </c>
+      <c r="N41" s="13">
+        <v>4.1152639999999998</v>
+      </c>
+      <c r="O41" s="13">
+        <v>2.9371160000000001</v>
+      </c>
+      <c r="P41" s="13">
+        <v>4.1176490000000001</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="8" type="noConversion"/>
+  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{32EB6AD7-BBCF-41A4-A705-09A536484B28}">
   <dimension ref="A1:A39"/>
   <sheetViews>

</xml_diff>

<commit_message>
Computing results, renaming get_log and get_quarterly scripts, organization changes
</commit_message>
<xml_diff>
--- a/Data Info/DadosEscolhidos.xlsx
+++ b/Data Info/DadosEscolhidos.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/ad5e0ae908eb1af8/Documentos/GitHub/gdp-forecasting-with-ML/Data Info/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="2225" documentId="11_AD4D361C20488DEA4E38A0E30418638E5BDEDD8E" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{58D1A83B-A3FC-4368-8EC0-C5C76B38FE96}"/>
+  <xr:revisionPtr revIDLastSave="2401" documentId="11_AD4D361C20488DEA4E38A0E30418638E5BDEDD8E" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{9BE02FB7-C322-49F9-A54B-FB93B901241F}"/>
   <bookViews>
     <workbookView xWindow="-45" yWindow="-16320" windowWidth="29040" windowHeight="15720" firstSheet="2" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -46,7 +46,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6303" uniqueCount="630">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6358" uniqueCount="642">
   <si>
     <t>NSAprod_cam_br</t>
   </si>
@@ -1929,30 +1929,6 @@
     <t># h=12</t>
   </si>
   <si>
-    <t>6 monthly, 6 quarterly</t>
-  </si>
-  <si>
-    <t>title h = 1</t>
-  </si>
-  <si>
-    <t>title h=12</t>
-  </si>
-  <si>
-    <t>half legend</t>
-  </si>
-  <si>
-    <t>other half, no leg title</t>
-  </si>
-  <si>
-    <t>lasso</t>
-  </si>
-  <si>
-    <t>enet</t>
-  </si>
-  <si>
-    <t>rf</t>
-  </si>
-  <si>
     <t>benchmark</t>
   </si>
   <si>
@@ -1965,22 +1941,84 @@
     <t>rf_model</t>
   </si>
   <si>
-    <t>rf_model2w</t>
-  </si>
-  <si>
     <t>datasetm</t>
   </si>
   <si>
     <t>old log, seas nsdiffs</t>
+  </si>
+  <si>
+    <t>rf_model1w</t>
+  </si>
+  <si>
+    <t>LASSO</t>
+  </si>
+  <si>
+    <t>Elastic Net</t>
+  </si>
+  <si>
+    <t>Random Forest</t>
+  </si>
+  <si>
+    <t>rRMSE</t>
+  </si>
+  <si>
+    <t>Quarterly analysis</t>
+  </si>
+  <si>
+    <t>Monthly analysis</t>
+  </si>
+  <si>
+    <t>Horizon 1</t>
+  </si>
+  <si>
+    <t>Horizon 4</t>
+  </si>
+  <si>
+    <t>Horizon 12</t>
+  </si>
+  <si>
+    <t>Benchmark</t>
+  </si>
+  <si>
+    <t>RF_model3q</t>
+  </si>
+  <si>
+    <t>1st option</t>
+  </si>
+  <si>
+    <t>2nd option</t>
+  </si>
+  <si>
+    <t>RMSE</t>
+  </si>
+  <si>
+    <t>"2.858255e-04***"</t>
+  </si>
+  <si>
+    <t>"7.452197e-04***"</t>
+  </si>
+  <si>
+    <t>"3.311928e-03**"</t>
+  </si>
+  <si>
+    <t>"5.831510e-05***"</t>
+  </si>
+  <si>
+    <t>"9.126611e-03**"</t>
+  </si>
+  <si>
+    <t>"2.155552e-07***"</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="2">
-    <numFmt numFmtId="170" formatCode="#,##0.0000"/>
-    <numFmt numFmtId="181" formatCode="0.0000"/>
+  <numFmts count="4">
+    <numFmt numFmtId="164" formatCode="#,##0.0000"/>
+    <numFmt numFmtId="165" formatCode="0.0000"/>
+    <numFmt numFmtId="167" formatCode="0.000"/>
+    <numFmt numFmtId="174" formatCode="#,##0.000"/>
   </numFmts>
   <fonts count="9" x14ac:knownFonts="1">
     <font>
@@ -2043,7 +2081,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="7">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -2080,6 +2118,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="2">
     <border>
@@ -2104,7 +2148,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="25">
+  <cellXfs count="32">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -2126,14 +2170,13 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="4" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="170" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="170" fontId="7" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="4" fontId="7" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -2146,20 +2189,38 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="170" fontId="7" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="7" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="170" fontId="7" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="7" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="170" fontId="7" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="7" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="170" fontId="7" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="7" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="181" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="7" fillId="7" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="4" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="4" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="174" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -23567,10 +23628,10 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3870FAA5-0C9A-4077-820D-651F982FFC52}">
-  <dimension ref="H3:Y41"/>
+  <dimension ref="H3:AI48"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D13" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="Q25" sqref="Q25"/>
+    <sheetView tabSelected="1" zoomScale="105" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="Q20" sqref="Q20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -23578,6 +23639,7 @@
     <col min="11" max="11" width="8.81640625" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="9.54296875" bestFit="1" customWidth="1"/>
     <col min="13" max="16" width="8.81640625" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="13" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="3" spans="8:22" x14ac:dyDescent="0.35">
@@ -23625,22 +23687,22 @@
         <v>574</v>
       </c>
       <c r="J5" s="10"/>
-      <c r="K5" s="15">
+      <c r="K5" s="14">
         <v>10.138339999999999</v>
       </c>
-      <c r="L5" s="15">
+      <c r="L5" s="14">
         <v>11.06123</v>
       </c>
-      <c r="M5" s="15">
+      <c r="M5" s="14">
         <v>7.387079</v>
       </c>
-      <c r="N5" s="15">
+      <c r="N5" s="14">
         <v>7.043361</v>
       </c>
-      <c r="O5" s="15">
+      <c r="O5" s="14">
         <v>5.4638929999999997</v>
       </c>
-      <c r="P5" s="15">
+      <c r="P5" s="14">
         <v>5.0934699999999999</v>
       </c>
       <c r="Q5" t="s">
@@ -23648,50 +23710,48 @@
       </c>
     </row>
     <row r="6" spans="8:22" x14ac:dyDescent="0.35">
-      <c r="I6" s="11" t="s">
+      <c r="I6" t="s">
         <v>573</v>
       </c>
-      <c r="J6" s="11"/>
-      <c r="K6" s="16">
+      <c r="K6" s="15">
         <v>5.3373280000000003</v>
       </c>
-      <c r="L6" s="12">
+      <c r="L6" s="11">
         <v>8.0436940000000003</v>
       </c>
-      <c r="M6" s="12">
+      <c r="M6" s="11">
         <v>4.3954370000000003</v>
       </c>
-      <c r="N6" s="12">
+      <c r="N6" s="11">
         <v>6.2554879999999997</v>
       </c>
-      <c r="O6" s="12">
+      <c r="O6" s="11">
         <v>3.273847</v>
       </c>
-      <c r="P6" s="12">
+      <c r="P6" s="11">
         <v>4.6032760000000001</v>
       </c>
     </row>
     <row r="7" spans="8:22" x14ac:dyDescent="0.35">
-      <c r="I7" s="11" t="s">
+      <c r="I7" t="s">
         <v>575</v>
       </c>
-      <c r="J7" s="11"/>
-      <c r="K7" s="17">
+      <c r="K7" s="16">
         <v>5.5069629999999998</v>
       </c>
-      <c r="L7" s="12">
+      <c r="L7" s="11">
         <v>7.9476279999999999</v>
       </c>
-      <c r="M7" s="17">
+      <c r="M7" s="16">
         <v>4.2647430000000002</v>
       </c>
-      <c r="N7" s="12">
+      <c r="N7" s="11">
         <v>6.2991429999999999</v>
       </c>
-      <c r="O7" s="17">
+      <c r="O7" s="16">
         <v>3.1697690000000001</v>
       </c>
-      <c r="P7" s="12">
+      <c r="P7" s="11">
         <v>4.6444510000000001</v>
       </c>
     </row>
@@ -23700,22 +23760,22 @@
         <v>581</v>
       </c>
       <c r="J8" s="10"/>
-      <c r="K8" s="15">
+      <c r="K8" s="14">
         <v>10.138339999999999</v>
       </c>
-      <c r="L8" s="15">
+      <c r="L8" s="14">
         <v>11.06123</v>
       </c>
-      <c r="M8" s="15">
+      <c r="M8" s="14">
         <v>7.387079</v>
       </c>
-      <c r="N8" s="15">
+      <c r="N8" s="14">
         <v>7.043361</v>
       </c>
-      <c r="O8" s="15">
+      <c r="O8" s="14">
         <v>5.4638929999999997</v>
       </c>
-      <c r="P8" s="15">
+      <c r="P8" s="14">
         <v>5.0934699999999999</v>
       </c>
       <c r="Q8" t="s">
@@ -23723,280 +23783,322 @@
       </c>
     </row>
     <row r="9" spans="8:22" x14ac:dyDescent="0.35">
-      <c r="I9" s="11" t="s">
+      <c r="I9" t="s">
         <v>582</v>
       </c>
-      <c r="J9" s="11"/>
-      <c r="K9" s="12">
+      <c r="K9" s="11">
         <v>5.3612840000000004</v>
       </c>
-      <c r="L9" s="12">
+      <c r="L9" s="11">
         <v>7.6462380000000003</v>
       </c>
-      <c r="M9" s="16">
+      <c r="M9" s="15">
         <v>4.273517</v>
       </c>
-      <c r="N9" s="12">
+      <c r="N9" s="11">
         <v>5.8681039999999998</v>
       </c>
-      <c r="O9" s="16">
+      <c r="O9" s="15">
         <v>3.1899090000000001</v>
       </c>
-      <c r="P9" s="12">
+      <c r="P9" s="11">
         <v>4.3203310000000004</v>
       </c>
     </row>
     <row r="10" spans="8:22" x14ac:dyDescent="0.35">
-      <c r="I10" s="11" t="s">
+      <c r="I10" t="s">
         <v>583</v>
       </c>
-      <c r="J10" s="11"/>
-      <c r="K10" s="12">
+      <c r="K10" s="11">
         <v>5.9704059999999997</v>
       </c>
-      <c r="L10" s="17">
+      <c r="L10" s="16">
         <v>7.6325320000000003</v>
       </c>
-      <c r="M10" s="12">
+      <c r="M10" s="11">
         <v>4.5451629999999996</v>
       </c>
-      <c r="N10" s="17">
+      <c r="N10" s="16">
         <v>5.8982469999999996</v>
       </c>
-      <c r="O10" s="12">
+      <c r="O10" s="11">
         <v>3.3889990000000001</v>
       </c>
-      <c r="P10" s="17">
+      <c r="P10" s="16">
         <v>4.3434660000000003</v>
       </c>
     </row>
     <row r="11" spans="8:22" x14ac:dyDescent="0.35">
-      <c r="H11" s="18"/>
+      <c r="H11" s="17"/>
       <c r="I11" s="10" t="s">
         <v>584</v>
       </c>
       <c r="J11" s="10"/>
-      <c r="K11" s="15">
+      <c r="K11" s="14">
         <v>10.138339999999999</v>
       </c>
-      <c r="L11" s="15">
+      <c r="L11" s="14">
         <v>11.06123</v>
       </c>
-      <c r="M11" s="15">
+      <c r="M11" s="14">
         <v>7.387079</v>
       </c>
-      <c r="N11" s="15">
+      <c r="N11" s="14">
         <v>7.043361</v>
       </c>
-      <c r="O11" s="15">
+      <c r="O11" s="14">
         <v>5.4638929999999997</v>
       </c>
-      <c r="P11" s="15">
+      <c r="P11" s="14">
         <v>5.0934699999999999</v>
       </c>
       <c r="Q11" t="s">
         <v>595</v>
       </c>
-      <c r="V11" s="18"/>
+      <c r="V11" s="17"/>
     </row>
     <row r="12" spans="8:22" x14ac:dyDescent="0.35">
-      <c r="H12" s="18"/>
-      <c r="I12" s="11" t="s">
+      <c r="H12" s="17"/>
+      <c r="I12" t="s">
         <v>585</v>
       </c>
-      <c r="J12" s="11"/>
-      <c r="K12" s="12">
+      <c r="K12" s="11">
         <v>5.3612840000000004</v>
       </c>
-      <c r="L12" s="12">
+      <c r="L12" s="11">
         <v>7.6462380000000003</v>
       </c>
-      <c r="M12" s="16">
+      <c r="M12" s="15">
         <v>4.273517</v>
       </c>
-      <c r="N12" s="12">
+      <c r="N12" s="11">
         <v>5.8681039999999998</v>
       </c>
-      <c r="O12" s="16">
+      <c r="O12" s="15">
         <v>3.1899090000000001</v>
       </c>
-      <c r="P12" s="12">
+      <c r="P12" s="11">
         <v>4.3203310000000004</v>
       </c>
-      <c r="V12" s="18"/>
+      <c r="V12" s="17"/>
     </row>
     <row r="13" spans="8:22" x14ac:dyDescent="0.35">
-      <c r="H13" s="18"/>
+      <c r="H13" s="17"/>
       <c r="I13" t="s">
         <v>586</v>
       </c>
-      <c r="K13" s="12">
+      <c r="K13" s="11">
         <v>5.9704059999999997</v>
       </c>
-      <c r="L13" s="17">
+      <c r="L13" s="16">
         <v>7.6325320000000003</v>
       </c>
-      <c r="M13" s="12">
+      <c r="M13" s="11">
         <v>4.5451629999999996</v>
       </c>
-      <c r="N13" s="17">
+      <c r="N13" s="16">
         <v>5.8982469999999996</v>
       </c>
-      <c r="O13" s="12">
+      <c r="O13" s="11">
         <v>3.3889990000000001</v>
       </c>
-      <c r="P13" s="17">
+      <c r="P13" s="16">
         <v>4.3434660000000003</v>
       </c>
-      <c r="V13" s="18"/>
+      <c r="V13" s="17"/>
     </row>
     <row r="14" spans="8:22" x14ac:dyDescent="0.35">
-      <c r="I14" s="10" t="s">
+      <c r="I14" t="s">
+        <v>632</v>
+      </c>
+      <c r="K14" s="11">
+        <v>7.4797289999999998</v>
+      </c>
+      <c r="L14" s="11">
+        <v>7.5066800000000002</v>
+      </c>
+      <c r="M14" s="26"/>
+      <c r="N14" s="26"/>
+      <c r="O14" s="11">
+        <v>3.3251400000000002</v>
+      </c>
+      <c r="P14" s="11">
+        <v>4.095269</v>
+      </c>
+    </row>
+    <row r="15" spans="8:22" x14ac:dyDescent="0.35">
+      <c r="I15" s="10" t="s">
         <v>587</v>
       </c>
-      <c r="J14" s="10"/>
-      <c r="K14" s="15">
+      <c r="J15" s="10"/>
+      <c r="K15" s="14">
         <v>10.138339999999999</v>
       </c>
-      <c r="L14" s="15">
+      <c r="L15" s="14">
         <v>11.06123</v>
       </c>
-      <c r="M14" s="15">
+      <c r="M15" s="14">
         <v>7.387079</v>
       </c>
-      <c r="N14" s="15">
+      <c r="N15" s="14">
         <v>7.043361</v>
       </c>
-      <c r="O14" s="15">
+      <c r="O15" s="14">
         <v>5.4638929999999997</v>
       </c>
-      <c r="P14" s="15">
+      <c r="P15" s="14">
         <v>5.0934699999999999</v>
       </c>
-      <c r="Q14" t="s">
+      <c r="Q15" t="s">
         <v>596</v>
-      </c>
-    </row>
-    <row r="15" spans="8:22" x14ac:dyDescent="0.35">
-      <c r="I15" t="s">
-        <v>588</v>
-      </c>
-      <c r="K15" s="12">
-        <v>5.4057740000000001</v>
-      </c>
-      <c r="L15" s="16">
-        <v>7.6163400000000001</v>
-      </c>
-      <c r="M15" s="12">
-        <v>4.3369090000000003</v>
-      </c>
-      <c r="N15" s="16">
-        <v>5.8291069999999996</v>
-      </c>
-      <c r="O15" s="12">
-        <v>3.2369050000000001</v>
-      </c>
-      <c r="P15" s="16">
-        <v>4.291474</v>
       </c>
     </row>
     <row r="16" spans="8:22" x14ac:dyDescent="0.35">
       <c r="I16" t="s">
+        <v>588</v>
+      </c>
+      <c r="K16" s="11">
+        <v>5.4057740000000001</v>
+      </c>
+      <c r="L16" s="15">
+        <v>7.6163400000000001</v>
+      </c>
+      <c r="M16" s="11">
+        <v>4.3369090000000003</v>
+      </c>
+      <c r="N16" s="15">
+        <v>5.8291069999999996</v>
+      </c>
+      <c r="O16" s="11">
+        <v>3.2369050000000001</v>
+      </c>
+      <c r="P16" s="15">
+        <v>4.291474</v>
+      </c>
+    </row>
+    <row r="17" spans="8:35" x14ac:dyDescent="0.35">
+      <c r="I17" t="s">
         <v>589</v>
       </c>
-      <c r="K16" s="12">
+      <c r="K17" s="11">
         <v>5.9582610000000003</v>
       </c>
-      <c r="L16" s="12">
+      <c r="L17" s="11">
         <v>7.656339</v>
       </c>
-      <c r="M16" s="12">
+      <c r="M17" s="11">
         <v>4.5040079999999998</v>
       </c>
-      <c r="N16" s="12">
+      <c r="N17" s="11">
         <v>5.9440749999999998</v>
       </c>
-      <c r="O16" s="12">
+      <c r="O17" s="11">
         <v>3.3588460000000002</v>
       </c>
-      <c r="P16" s="12">
+      <c r="P17" s="11">
         <v>4.3810200000000004</v>
       </c>
     </row>
-    <row r="17" spans="8:25" x14ac:dyDescent="0.35">
-      <c r="I17" s="10" t="s">
+    <row r="18" spans="8:35" x14ac:dyDescent="0.35">
+      <c r="I18" s="10" t="s">
         <v>590</v>
       </c>
-      <c r="J17" s="10"/>
-      <c r="K17" s="15">
+      <c r="J18" s="10"/>
+      <c r="K18" s="14">
         <v>10.138339999999999</v>
       </c>
-      <c r="L17" s="15">
+      <c r="L18" s="14">
         <v>11.06123</v>
       </c>
-      <c r="M17" s="15">
+      <c r="M18" s="14">
         <v>7.387079</v>
       </c>
-      <c r="N17" s="15">
+      <c r="N18" s="14">
         <v>7.043361</v>
       </c>
-      <c r="O17" s="15">
+      <c r="O18" s="14">
         <v>5.4638929999999997</v>
       </c>
-      <c r="P17" s="15">
+      <c r="P18" s="14">
         <v>5.0934699999999999</v>
       </c>
-      <c r="Q17" t="s">
+      <c r="Q18" t="s">
         <v>597</v>
       </c>
-    </row>
-    <row r="18" spans="8:25" x14ac:dyDescent="0.35">
-      <c r="I18" t="s">
+      <c r="X18" t="s">
+        <v>633</v>
+      </c>
+    </row>
+    <row r="19" spans="8:35" x14ac:dyDescent="0.35">
+      <c r="I19" t="s">
         <v>591</v>
       </c>
-      <c r="K18" s="12">
+      <c r="K19" s="11">
         <v>5.4057740000000001</v>
       </c>
-      <c r="L18" s="16">
+      <c r="L19" s="15">
         <v>7.6163400000000001</v>
       </c>
-      <c r="M18" s="12">
+      <c r="M19" s="11">
         <v>4.3369090000000003</v>
       </c>
-      <c r="N18" s="16">
+      <c r="N19" s="15">
         <v>5.8291069999999996</v>
       </c>
-      <c r="O18" s="12">
+      <c r="O19" s="11">
         <v>3.2369050000000001</v>
       </c>
-      <c r="P18" s="16">
+      <c r="P19" s="15">
         <v>4.291474</v>
       </c>
     </row>
-    <row r="19" spans="8:25" x14ac:dyDescent="0.35">
-      <c r="I19" t="s">
+    <row r="20" spans="8:35" x14ac:dyDescent="0.35">
+      <c r="I20" t="s">
         <v>592</v>
       </c>
-      <c r="K19" s="12">
+      <c r="K20" s="11">
         <v>5.9582610000000003</v>
       </c>
-      <c r="L19" s="12">
+      <c r="L20" s="11">
         <v>7.656339</v>
       </c>
-      <c r="M19" s="12">
+      <c r="M20" s="11">
         <v>4.5040079999999998</v>
       </c>
-      <c r="N19" s="12">
+      <c r="N20" s="11">
         <v>5.9440749999999998</v>
       </c>
-      <c r="O19" s="12">
+      <c r="O20" s="11">
         <v>3.3588460000000002</v>
       </c>
-      <c r="P19" s="12">
+      <c r="P20" s="11">
         <v>4.3810200000000004</v>
       </c>
-    </row>
-    <row r="22" spans="8:25" x14ac:dyDescent="0.35">
+      <c r="X20" t="s">
+        <v>580</v>
+      </c>
+      <c r="Y20" t="s">
+        <v>626</v>
+      </c>
+      <c r="AA20" t="s">
+        <v>627</v>
+      </c>
+    </row>
+    <row r="21" spans="8:35" x14ac:dyDescent="0.35">
+      <c r="Y21" t="s">
+        <v>628</v>
+      </c>
+      <c r="Z21" t="s">
+        <v>629</v>
+      </c>
+      <c r="AA21" t="s">
+        <v>628</v>
+      </c>
+      <c r="AB21" t="s">
+        <v>630</v>
+      </c>
+    </row>
+    <row r="22" spans="8:35" x14ac:dyDescent="0.35">
       <c r="K22" t="s">
         <v>576</v>
       </c>
@@ -24016,10 +24118,26 @@
         <v>614</v>
       </c>
       <c r="X22" t="s">
-        <v>615</v>
-      </c>
-    </row>
-    <row r="23" spans="8:25" x14ac:dyDescent="0.35">
+        <v>631</v>
+      </c>
+      <c r="Y22" s="27" t="str">
+        <f>ROUND(O11,2)&amp;"%"</f>
+        <v>5,46%</v>
+      </c>
+      <c r="Z22" s="27" t="str">
+        <f>ROUND(P11,2)&amp;"%"</f>
+        <v>5,09%</v>
+      </c>
+      <c r="AA22" s="27" t="str">
+        <f>ROUND(O28,2)&amp;"%"</f>
+        <v>1,08%</v>
+      </c>
+      <c r="AB22" s="27" t="str">
+        <f>ROUND(P28,2)&amp;"%"</f>
+        <v>1,48%</v>
+      </c>
+    </row>
+    <row r="23" spans="8:35" x14ac:dyDescent="0.35">
       <c r="K23" t="s">
         <v>578</v>
       </c>
@@ -24038,433 +24156,909 @@
       <c r="P23" t="s">
         <v>580</v>
       </c>
-    </row>
-    <row r="24" spans="8:25" x14ac:dyDescent="0.35">
+      <c r="X23" t="s">
+        <v>622</v>
+      </c>
+      <c r="Y23" s="27" t="str">
+        <f>ROUND(O12,2)&amp;"%"</f>
+        <v>3,19%</v>
+      </c>
+      <c r="Z23" s="27" t="str">
+        <f>ROUND(P12,2)&amp;"%"</f>
+        <v>4,32%</v>
+      </c>
+      <c r="AA23" s="27" t="str">
+        <f>ROUND(O29,2)&amp;"%"</f>
+        <v>0,59%</v>
+      </c>
+      <c r="AB23" s="27" t="str">
+        <f>ROUND(P29,2)&amp;"%"</f>
+        <v>0,91%</v>
+      </c>
+    </row>
+    <row r="24" spans="8:35" x14ac:dyDescent="0.35">
       <c r="I24" t="s">
+        <v>615</v>
+      </c>
+      <c r="K24" s="18">
+        <v>6.6295580000000007E-2</v>
+      </c>
+      <c r="L24" s="12">
+        <v>9.8374290000000003E-2</v>
+      </c>
+      <c r="M24" s="18">
+        <v>4.8804380000000001E-2</v>
+      </c>
+      <c r="N24" s="12">
+        <v>7.0079680000000005E-2</v>
+      </c>
+      <c r="O24" s="18">
+        <v>1.048171</v>
+      </c>
+      <c r="P24" s="12">
+        <v>1.5017780000000001</v>
+      </c>
+      <c r="Q24" t="s">
+        <v>619</v>
+      </c>
+      <c r="R24" t="s">
+        <v>620</v>
+      </c>
+      <c r="X24" t="s">
         <v>623</v>
       </c>
-      <c r="K24" s="19">
-        <v>6.6295580000000007E-2</v>
-      </c>
-      <c r="L24" s="13">
-        <v>9.8374290000000003E-2</v>
-      </c>
-      <c r="M24" s="19">
-        <v>4.8804380000000001E-2</v>
-      </c>
-      <c r="N24" s="13">
-        <v>7.0079680000000005E-2</v>
-      </c>
-      <c r="O24" s="19">
-        <v>1.048171</v>
-      </c>
-      <c r="P24" s="13">
-        <v>1.5017780000000001</v>
-      </c>
-      <c r="Q24" t="s">
-        <v>628</v>
-      </c>
-      <c r="R24" t="s">
-        <v>629</v>
-      </c>
-    </row>
-    <row r="25" spans="8:25" x14ac:dyDescent="0.35">
+      <c r="Y24" s="27" t="str">
+        <f>ROUND(O13,2)&amp;"%"</f>
+        <v>3,39%</v>
+      </c>
+      <c r="Z24" s="27" t="str">
+        <f>ROUND(P13,2)&amp;"%"</f>
+        <v>4,34%</v>
+      </c>
+      <c r="AA24" s="27" t="str">
+        <f>ROUND(O30,2)&amp;"%"</f>
+        <v>0,81%</v>
+      </c>
+      <c r="AB24" s="27" t="str">
+        <f>ROUND(P30,2)&amp;"%"</f>
+        <v>1,08%</v>
+      </c>
+    </row>
+    <row r="25" spans="8:35" x14ac:dyDescent="0.35">
       <c r="I25" t="s">
+        <v>616</v>
+      </c>
+      <c r="K25" s="12">
+        <v>3.6495979999999997E-2</v>
+      </c>
+      <c r="L25" s="12">
+        <v>5.9897640000000002E-2</v>
+      </c>
+      <c r="M25" s="12">
+        <v>2.8393020000000001E-2</v>
+      </c>
+      <c r="N25" s="12">
+        <v>4.3121090000000001E-2</v>
+      </c>
+      <c r="O25" s="12">
+        <v>0.61500900000000003</v>
+      </c>
+      <c r="P25" s="12">
+        <v>0.93870880000000001</v>
+      </c>
+      <c r="X25" t="s">
         <v>624</v>
       </c>
-      <c r="K25" s="13">
-        <v>3.6495979999999997E-2</v>
-      </c>
-      <c r="L25" s="13">
-        <v>5.9897640000000002E-2</v>
-      </c>
-      <c r="M25" s="13">
-        <v>2.8393020000000001E-2</v>
-      </c>
-      <c r="N25" s="13">
-        <v>4.3121090000000001E-2</v>
-      </c>
-      <c r="O25" s="13">
-        <v>0.61500900000000003</v>
-      </c>
-      <c r="P25" s="13">
-        <v>0.93870880000000001</v>
-      </c>
-    </row>
-    <row r="26" spans="8:25" x14ac:dyDescent="0.35">
+      <c r="Y25" s="27" t="str">
+        <f>ROUND(O14,2)&amp;"%"</f>
+        <v>3,33%</v>
+      </c>
+      <c r="Z25" s="27" t="str">
+        <f>ROUND(P14,2)&amp;"%"</f>
+        <v>4,1%</v>
+      </c>
+      <c r="AA25" s="27" t="str">
+        <f>ROUND(O31,2)&amp;"%"</f>
+        <v>0,73%</v>
+      </c>
+      <c r="AB25" s="27" t="str">
+        <f>ROUND(P31,2)&amp;"%"</f>
+        <v>0,85%</v>
+      </c>
+    </row>
+    <row r="26" spans="8:35" x14ac:dyDescent="0.35">
       <c r="I26" t="s">
+        <v>617</v>
+      </c>
+      <c r="K26" s="12">
+        <v>5.0724129999999999E-2</v>
+      </c>
+      <c r="L26" s="12">
+        <v>6.4122650000000003E-2</v>
+      </c>
+      <c r="M26" s="12">
+        <v>3.893112E-2</v>
+      </c>
+      <c r="N26" s="12">
+        <v>5.13068E-2</v>
+      </c>
+      <c r="O26" s="12">
+        <v>0.83906159999999996</v>
+      </c>
+      <c r="P26" s="12">
+        <v>1.1120433000000001</v>
+      </c>
+    </row>
+    <row r="27" spans="8:35" x14ac:dyDescent="0.35">
+      <c r="I27" t="s">
+        <v>618</v>
+      </c>
+      <c r="K27" s="23">
+        <v>5.0135369999999999E-2</v>
+      </c>
+      <c r="L27" s="23">
+        <v>5.4280870000000002E-2</v>
+      </c>
+      <c r="M27" s="23">
+        <v>3.5086409999999998E-2</v>
+      </c>
+      <c r="N27" s="23">
+        <v>4.0220220000000001E-2</v>
+      </c>
+      <c r="O27" s="23">
+        <v>0.75690360000000001</v>
+      </c>
+      <c r="P27" s="23">
+        <v>0.86743199999999998</v>
+      </c>
+      <c r="X27" t="s">
         <v>625</v>
       </c>
-      <c r="K26" s="13">
-        <v>5.0724129999999999E-2</v>
-      </c>
-      <c r="L26" s="13">
-        <v>6.4122650000000003E-2</v>
-      </c>
-      <c r="M26" s="13">
-        <v>3.893112E-2</v>
-      </c>
-      <c r="N26" s="13">
-        <v>5.13068E-2</v>
-      </c>
-      <c r="O26" s="13">
-        <v>0.83906159999999996</v>
-      </c>
-      <c r="P26" s="13">
-        <v>1.1120433000000001</v>
-      </c>
-      <c r="X26" t="s">
-        <v>616</v>
-      </c>
-      <c r="Y26" t="s">
-        <v>617</v>
-      </c>
-    </row>
-    <row r="27" spans="8:25" x14ac:dyDescent="0.35">
-      <c r="I27" t="s">
+      <c r="Y27" t="s">
         <v>626</v>
       </c>
-      <c r="K27" s="24">
-        <v>5.0135369999999999E-2</v>
-      </c>
-      <c r="L27" s="24">
-        <v>5.4280870000000002E-2</v>
-      </c>
-      <c r="M27" s="24">
-        <v>3.5086409999999998E-2</v>
-      </c>
-      <c r="N27" s="24">
-        <v>4.0220220000000001E-2</v>
-      </c>
-      <c r="O27" s="24">
-        <v>0.75690360000000001</v>
-      </c>
-      <c r="P27" s="24">
-        <v>0.86743199999999998</v>
-      </c>
-      <c r="X27" s="18" t="s">
-        <v>620</v>
-      </c>
-      <c r="Y27" s="18"/>
-    </row>
-    <row r="28" spans="8:25" x14ac:dyDescent="0.35">
-      <c r="H28" s="23"/>
+      <c r="AA27" t="s">
+        <v>627</v>
+      </c>
+      <c r="AD27" t="s">
+        <v>635</v>
+      </c>
+      <c r="AE27" t="s">
+        <v>626</v>
+      </c>
+      <c r="AG27" t="s">
+        <v>627</v>
+      </c>
+    </row>
+    <row r="28" spans="8:35" x14ac:dyDescent="0.35">
+      <c r="H28" s="22"/>
       <c r="I28" s="10" t="s">
         <v>602</v>
       </c>
       <c r="J28" s="10"/>
-      <c r="K28" s="14">
+      <c r="K28" s="13">
         <v>6.7389569999999996E-2</v>
       </c>
-      <c r="L28" s="20">
+      <c r="L28" s="19">
         <v>9.6357360000000003E-2</v>
       </c>
-      <c r="M28" s="14">
+      <c r="M28" s="13">
         <v>5.007342E-2</v>
       </c>
-      <c r="N28" s="20">
+      <c r="N28" s="19">
         <v>6.8928249999999996E-2</v>
       </c>
-      <c r="O28" s="14">
+      <c r="O28" s="13">
         <v>1.0766389999999999</v>
       </c>
-      <c r="P28" s="20">
+      <c r="P28" s="19">
         <v>1.4784839999999999</v>
       </c>
       <c r="Q28" t="s">
         <v>598</v>
       </c>
-      <c r="U28" s="23"/>
-      <c r="X28" s="18" t="s">
-        <v>621</v>
-      </c>
-      <c r="Y28" s="18"/>
-    </row>
-    <row r="29" spans="8:25" x14ac:dyDescent="0.35">
-      <c r="H29" s="23"/>
+      <c r="U28" s="22"/>
+      <c r="Y28" t="s">
+        <v>628</v>
+      </c>
+      <c r="Z28" t="s">
+        <v>629</v>
+      </c>
+      <c r="AA28" t="s">
+        <v>628</v>
+      </c>
+      <c r="AB28" t="s">
+        <v>630</v>
+      </c>
+      <c r="AE28" t="s">
+        <v>628</v>
+      </c>
+      <c r="AF28" t="s">
+        <v>629</v>
+      </c>
+      <c r="AG28" t="s">
+        <v>628</v>
+      </c>
+      <c r="AH28" t="s">
+        <v>630</v>
+      </c>
+    </row>
+    <row r="29" spans="8:35" x14ac:dyDescent="0.35">
+      <c r="H29" s="22"/>
       <c r="I29" t="s">
         <v>603</v>
       </c>
-      <c r="K29" s="21">
+      <c r="K29" s="20">
         <v>3.5456799999999997E-2</v>
       </c>
-      <c r="L29" s="21">
+      <c r="L29" s="20">
         <v>5.7688940000000001E-2</v>
       </c>
-      <c r="M29" s="21">
+      <c r="M29" s="20">
         <v>2.732362E-2</v>
       </c>
-      <c r="N29" s="21">
+      <c r="N29" s="20">
         <v>4.1704409999999997E-2</v>
       </c>
-      <c r="O29" s="21">
+      <c r="O29" s="20">
         <v>0.59215430000000002</v>
       </c>
-      <c r="P29" s="21">
+      <c r="P29" s="20">
         <v>0.90730739999999999</v>
       </c>
-      <c r="U29" s="23"/>
-      <c r="X29" s="18" t="s">
-        <v>622</v>
-      </c>
-      <c r="Y29" s="18"/>
-    </row>
-    <row r="30" spans="8:25" x14ac:dyDescent="0.35">
-      <c r="H30" s="23"/>
+      <c r="U29" s="22"/>
+      <c r="X29" t="s">
+        <v>631</v>
+      </c>
+      <c r="Y29" s="25">
+        <v>1</v>
+      </c>
+      <c r="Z29" s="25">
+        <v>1</v>
+      </c>
+      <c r="AA29" s="25">
+        <v>1</v>
+      </c>
+      <c r="AB29" s="25">
+        <v>1</v>
+      </c>
+      <c r="AD29" t="s">
+        <v>631</v>
+      </c>
+      <c r="AE29" s="29">
+        <f>K11</f>
+        <v>10.138339999999999</v>
+      </c>
+      <c r="AF29" s="29">
+        <f>L11</f>
+        <v>11.06123</v>
+      </c>
+      <c r="AG29" s="29">
+        <f>K28</f>
+        <v>6.7389569999999996E-2</v>
+      </c>
+      <c r="AH29" s="29">
+        <f>L28</f>
+        <v>9.6357360000000003E-2</v>
+      </c>
+      <c r="AI29" s="29"/>
+    </row>
+    <row r="30" spans="8:35" x14ac:dyDescent="0.35">
+      <c r="H30" s="22"/>
       <c r="I30" t="s">
         <v>604</v>
       </c>
-      <c r="K30" s="22">
+      <c r="K30" s="21">
         <v>4.9312519999999999E-2</v>
       </c>
-      <c r="L30" s="22">
+      <c r="L30" s="21">
         <v>6.2136660000000003E-2</v>
       </c>
-      <c r="M30" s="22">
+      <c r="M30" s="21">
         <v>3.7580210000000003E-2</v>
       </c>
-      <c r="N30" s="22">
+      <c r="N30" s="21">
         <v>4.9575040000000001E-2</v>
       </c>
-      <c r="O30" s="22">
+      <c r="O30" s="21">
         <v>0.81035729999999995</v>
       </c>
-      <c r="P30" s="22">
+      <c r="P30" s="21">
         <v>1.0750708</v>
       </c>
-      <c r="U30" s="23"/>
+      <c r="U30" s="22"/>
       <c r="X30" t="s">
-        <v>618</v>
-      </c>
-      <c r="Y30" t="s">
-        <v>619</v>
-      </c>
-    </row>
-    <row r="31" spans="8:25" x14ac:dyDescent="0.35">
-      <c r="I31" s="10" t="s">
+        <v>622</v>
+      </c>
+      <c r="Y30" s="25">
+        <f>K12/$K$11</f>
+        <v>0.52881280367397432</v>
+      </c>
+      <c r="Z30" s="25">
+        <f>L12/$L$11</f>
+        <v>0.69126471468362927</v>
+      </c>
+      <c r="AA30" s="25">
+        <f>K29/$K$28</f>
+        <v>0.5261467019302839</v>
+      </c>
+      <c r="AB30" s="25">
+        <f>L29/$L$28</f>
+        <v>0.59869780575142362</v>
+      </c>
+      <c r="AD30" t="s">
+        <v>622</v>
+      </c>
+      <c r="AE30" s="29">
+        <f t="shared" ref="AE30:AF30" si="0">K12</f>
+        <v>5.3612840000000004</v>
+      </c>
+      <c r="AF30" s="29">
+        <f t="shared" si="0"/>
+        <v>7.6462380000000003</v>
+      </c>
+      <c r="AG30" s="29">
+        <f t="shared" ref="AG30:AG32" si="1">K29</f>
+        <v>3.5456799999999997E-2</v>
+      </c>
+      <c r="AH30" s="29">
+        <f t="shared" ref="AH30:AH32" si="2">L29</f>
+        <v>5.7688940000000001E-2</v>
+      </c>
+      <c r="AI30" s="29"/>
+    </row>
+    <row r="31" spans="8:35" x14ac:dyDescent="0.35">
+      <c r="I31" t="s">
+        <v>621</v>
+      </c>
+      <c r="K31" s="24">
+        <v>4.8549160000000001E-2</v>
+      </c>
+      <c r="L31" s="24">
+        <v>5.3747389999999999E-2</v>
+      </c>
+      <c r="M31" s="24">
+        <v>3.3600360000000003E-2</v>
+      </c>
+      <c r="N31" s="24">
+        <v>3.9196839999999997E-2</v>
+      </c>
+      <c r="O31" s="24">
+        <v>0.72549490000000005</v>
+      </c>
+      <c r="P31" s="24">
+        <v>0.84613229999999995</v>
+      </c>
+      <c r="X31" t="s">
+        <v>623</v>
+      </c>
+      <c r="Y31" s="25">
+        <f>K13/$K$11</f>
+        <v>0.58889384258172439</v>
+      </c>
+      <c r="Z31" s="25">
+        <f>L13/$L$11</f>
+        <v>0.69002561197986123</v>
+      </c>
+      <c r="AA31" s="25">
+        <f>K30/$K$28</f>
+        <v>0.7317529997594584</v>
+      </c>
+      <c r="AB31" s="25">
+        <f>L30/$L$28</f>
+        <v>0.64485639706193698</v>
+      </c>
+      <c r="AD31" t="s">
+        <v>623</v>
+      </c>
+      <c r="AE31" s="29">
+        <f t="shared" ref="AE31:AF31" si="3">K13</f>
+        <v>5.9704059999999997</v>
+      </c>
+      <c r="AF31" s="29">
+        <f t="shared" si="3"/>
+        <v>7.6325320000000003</v>
+      </c>
+      <c r="AG31" s="29">
+        <f t="shared" si="1"/>
+        <v>4.9312519999999999E-2</v>
+      </c>
+      <c r="AH31" s="29">
+        <f t="shared" si="2"/>
+        <v>6.2136660000000003E-2</v>
+      </c>
+      <c r="AI31" s="29"/>
+    </row>
+    <row r="32" spans="8:35" x14ac:dyDescent="0.35">
+      <c r="I32" s="10" t="s">
         <v>605</v>
       </c>
-      <c r="J31" s="10"/>
-      <c r="K31" s="14">
+      <c r="J32" s="10"/>
+      <c r="K32" s="13">
         <v>6.7389569999999996E-2</v>
       </c>
-      <c r="L31" s="20">
+      <c r="L32" s="19">
         <v>9.6357360000000003E-2</v>
       </c>
-      <c r="M31" s="14">
+      <c r="M32" s="13">
         <v>5.007342E-2</v>
       </c>
-      <c r="N31" s="20">
+      <c r="N32" s="19">
         <v>6.8928249999999996E-2</v>
       </c>
-      <c r="O31" s="14">
+      <c r="O32" s="13">
         <v>1.0766389999999999</v>
       </c>
-      <c r="P31" s="20">
+      <c r="P32" s="19">
         <v>1.4784839999999999</v>
       </c>
-      <c r="Q31" t="s">
+      <c r="Q32" t="s">
         <v>599</v>
       </c>
-    </row>
-    <row r="32" spans="8:25" x14ac:dyDescent="0.35">
-      <c r="I32" t="s">
+      <c r="X32" t="s">
+        <v>624</v>
+      </c>
+      <c r="Y32" s="25">
+        <f>K14/$K$11</f>
+        <v>0.73776663635269679</v>
+      </c>
+      <c r="Z32" s="25">
+        <f>L14/$L$11</f>
+        <v>0.67864785381010972</v>
+      </c>
+      <c r="AA32" s="25">
+        <f>K31/$K$28</f>
+        <v>0.72042543081963584</v>
+      </c>
+      <c r="AB32" s="25">
+        <f>L31/$L$28</f>
+        <v>0.55779226413010896</v>
+      </c>
+      <c r="AD32" t="s">
+        <v>624</v>
+      </c>
+      <c r="AE32" s="29">
+        <f t="shared" ref="AE32:AF32" si="4">K14</f>
+        <v>7.4797289999999998</v>
+      </c>
+      <c r="AF32" s="29">
+        <f t="shared" si="4"/>
+        <v>7.5066800000000002</v>
+      </c>
+      <c r="AG32" s="29">
+        <f t="shared" si="1"/>
+        <v>4.8549160000000001E-2</v>
+      </c>
+      <c r="AH32" s="29">
+        <f t="shared" si="2"/>
+        <v>5.3747389999999999E-2</v>
+      </c>
+      <c r="AI32" s="29"/>
+    </row>
+    <row r="33" spans="9:32" x14ac:dyDescent="0.35">
+      <c r="I33" t="s">
         <v>606</v>
       </c>
-      <c r="K32" s="13">
+      <c r="K33" s="12">
         <v>0.10952291</v>
       </c>
-      <c r="L32" s="13">
+      <c r="L33" s="12">
         <v>6.3788289999999997E-2</v>
       </c>
-      <c r="M32" s="13">
+      <c r="M33" s="12">
         <v>4.4270120000000003E-2</v>
       </c>
-      <c r="N32" s="13">
+      <c r="N33" s="12">
         <v>4.4905760000000003E-2</v>
       </c>
-      <c r="O32" s="13">
+      <c r="O33" s="12">
         <v>0.96270840000000002</v>
       </c>
-      <c r="P32" s="13">
+      <c r="P33" s="12">
         <v>0.97586759999999995</v>
       </c>
     </row>
-    <row r="33" spans="9:17" x14ac:dyDescent="0.35">
-      <c r="I33" t="s">
+    <row r="34" spans="9:32" x14ac:dyDescent="0.35">
+      <c r="I34" t="s">
         <v>607</v>
       </c>
-      <c r="K33" s="13">
+      <c r="K34" s="12">
         <v>5.2181999999999999E-2</v>
       </c>
-      <c r="L33" s="13">
+      <c r="L34" s="12">
         <v>6.6322430000000002E-2</v>
       </c>
-      <c r="M33" s="13">
+      <c r="M34" s="12">
         <v>3.865532E-2</v>
       </c>
-      <c r="N33" s="13">
+      <c r="N34" s="12">
         <v>5.1502010000000001E-2</v>
       </c>
-      <c r="O33" s="13">
+      <c r="O34" s="12">
         <v>0.83366150000000006</v>
       </c>
-      <c r="P33" s="13">
+      <c r="P34" s="12">
         <v>1.1166924</v>
       </c>
-    </row>
-    <row r="34" spans="9:17" x14ac:dyDescent="0.35">
-      <c r="I34" t="s">
+      <c r="X34" t="s">
+        <v>634</v>
+      </c>
+    </row>
+    <row r="35" spans="9:32" x14ac:dyDescent="0.35">
+      <c r="Y35" s="28" t="s">
+        <v>626</v>
+      </c>
+      <c r="Z35" s="28"/>
+      <c r="AA35" s="28"/>
+      <c r="AB35" s="28"/>
+      <c r="AC35" s="28" t="s">
         <v>627</v>
       </c>
-    </row>
-    <row r="36" spans="9:17" x14ac:dyDescent="0.35">
+      <c r="AD35" s="28"/>
+      <c r="AE35" s="28"/>
+      <c r="AF35" s="28"/>
+    </row>
+    <row r="36" spans="9:32" x14ac:dyDescent="0.35">
       <c r="I36" s="10" t="s">
         <v>608</v>
       </c>
       <c r="J36" s="10"/>
-      <c r="K36" s="14">
+      <c r="K36" s="13">
         <v>7.3945249999999998</v>
       </c>
-      <c r="L36" s="14">
+      <c r="L36" s="13">
         <v>10.177414000000001</v>
       </c>
-      <c r="M36" s="14">
+      <c r="M36" s="13">
         <v>5.3058959999999997</v>
       </c>
-      <c r="N36" s="14">
+      <c r="N36" s="13">
         <v>7.203055</v>
       </c>
-      <c r="O36" s="14">
+      <c r="O36" s="13">
         <v>5.0400410000000004</v>
       </c>
-      <c r="P36" s="14">
+      <c r="P36" s="13">
         <v>6.8124219999999998</v>
       </c>
       <c r="Q36" t="s">
         <v>600</v>
       </c>
-    </row>
-    <row r="37" spans="9:17" x14ac:dyDescent="0.35">
+      <c r="Y36" s="28" t="s">
+        <v>628</v>
+      </c>
+      <c r="Z36" s="28"/>
+      <c r="AA36" s="28" t="s">
+        <v>629</v>
+      </c>
+      <c r="AB36" s="28"/>
+      <c r="AC36" s="28" t="s">
+        <v>628</v>
+      </c>
+      <c r="AD36" s="28"/>
+      <c r="AE36" s="28" t="s">
+        <v>630</v>
+      </c>
+      <c r="AF36" s="28"/>
+    </row>
+    <row r="37" spans="9:32" x14ac:dyDescent="0.35">
       <c r="I37" t="s">
         <v>609</v>
       </c>
-      <c r="K37" s="13">
+      <c r="K37" s="12">
         <v>3.7484489999999999</v>
       </c>
-      <c r="L37" s="13">
+      <c r="L37" s="12">
         <v>5.9246020000000001</v>
       </c>
-      <c r="M37" s="13">
+      <c r="M37" s="12">
         <v>2.8394059999999999</v>
       </c>
-      <c r="N37" s="13">
+      <c r="N37" s="12">
         <v>4.3051529999999998</v>
       </c>
-      <c r="O37" s="13">
+      <c r="O37" s="12">
         <v>2.7975469999999998</v>
       </c>
-      <c r="P37" s="13">
+      <c r="P37" s="12">
         <v>4.2833860000000001</v>
       </c>
-    </row>
-    <row r="38" spans="9:17" x14ac:dyDescent="0.35">
+      <c r="Y37" t="s">
+        <v>625</v>
+      </c>
+      <c r="Z37" t="s">
+        <v>580</v>
+      </c>
+      <c r="AA37" t="s">
+        <v>625</v>
+      </c>
+      <c r="AB37" t="s">
+        <v>580</v>
+      </c>
+      <c r="AC37" t="s">
+        <v>625</v>
+      </c>
+      <c r="AD37" t="s">
+        <v>580</v>
+      </c>
+      <c r="AE37" t="s">
+        <v>625</v>
+      </c>
+      <c r="AF37" t="s">
+        <v>580</v>
+      </c>
+    </row>
+    <row r="38" spans="9:32" x14ac:dyDescent="0.35">
       <c r="I38" t="s">
         <v>610</v>
       </c>
-      <c r="K38" s="13">
+      <c r="K38" s="12">
         <v>3.7453059999999998</v>
       </c>
-      <c r="L38" s="13">
+      <c r="L38" s="12">
         <v>5.4190430000000003</v>
       </c>
-      <c r="M38" s="13">
+      <c r="M38" s="12">
         <v>2.8651089999999999</v>
       </c>
-      <c r="N38" s="13">
+      <c r="N38" s="12">
         <v>3.8482769999999999</v>
       </c>
-      <c r="O38" s="13">
+      <c r="O38" s="12">
         <v>2.8197679999999998</v>
       </c>
-      <c r="P38" s="13">
+      <c r="P38" s="12">
         <v>3.8382869999999998</v>
       </c>
-    </row>
-    <row r="39" spans="9:17" x14ac:dyDescent="0.35">
+      <c r="X38" t="s">
+        <v>631</v>
+      </c>
+      <c r="Y38" s="25">
+        <v>1</v>
+      </c>
+      <c r="Z38" s="27" t="str">
+        <f>ROUND(O11,2)&amp;"%"</f>
+        <v>5,46%</v>
+      </c>
+      <c r="AA38" s="25">
+        <v>1</v>
+      </c>
+      <c r="AB38" s="27" t="str">
+        <f>ROUND(P11,2)&amp;"%"</f>
+        <v>5,09%</v>
+      </c>
+      <c r="AC38" s="25">
+        <v>1</v>
+      </c>
+      <c r="AD38" s="27" t="str">
+        <f>ROUND(O28,2)&amp;"%"</f>
+        <v>1,08%</v>
+      </c>
+      <c r="AE38" s="25">
+        <v>1</v>
+      </c>
+      <c r="AF38" s="27" t="str">
+        <f>ROUND(P28,2)&amp;"%"</f>
+        <v>1,48%</v>
+      </c>
+    </row>
+    <row r="39" spans="9:32" x14ac:dyDescent="0.35">
       <c r="I39" s="10" t="s">
         <v>611</v>
       </c>
       <c r="J39" s="10"/>
-      <c r="K39" s="14">
+      <c r="K39" s="13">
         <v>7.3865740000000004</v>
       </c>
-      <c r="L39" s="14">
+      <c r="L39" s="13">
         <v>10.201127</v>
       </c>
-      <c r="M39" s="14">
+      <c r="M39" s="13">
         <v>5.272157</v>
       </c>
-      <c r="N39" s="14">
+      <c r="N39" s="13">
         <v>7.1923769999999996</v>
       </c>
-      <c r="O39" s="14">
+      <c r="O39" s="13">
         <v>4.9960110000000002</v>
       </c>
-      <c r="P39" s="14">
+      <c r="P39" s="13">
         <v>6.7898480000000001</v>
       </c>
       <c r="Q39" t="s">
         <v>601</v>
       </c>
-    </row>
-    <row r="40" spans="9:17" x14ac:dyDescent="0.35">
+      <c r="X39" t="s">
+        <v>622</v>
+      </c>
+      <c r="Y39" s="25">
+        <v>0.52881280367397432</v>
+      </c>
+      <c r="Z39" s="27" t="str">
+        <f t="shared" ref="Z39:Z41" si="5">ROUND(O12,2)&amp;"%"</f>
+        <v>3,19%</v>
+      </c>
+      <c r="AA39" s="25">
+        <v>0.69126471468362927</v>
+      </c>
+      <c r="AB39" s="27" t="str">
+        <f t="shared" ref="AB39:AB41" si="6">ROUND(P12,2)&amp;"%"</f>
+        <v>4,32%</v>
+      </c>
+      <c r="AC39" s="25">
+        <v>0.5261467019302839</v>
+      </c>
+      <c r="AD39" s="27" t="str">
+        <f t="shared" ref="AD39:AD41" si="7">ROUND(O29,2)&amp;"%"</f>
+        <v>0,59%</v>
+      </c>
+      <c r="AE39" s="25">
+        <v>0.59869780575142362</v>
+      </c>
+      <c r="AF39" s="27" t="str">
+        <f t="shared" ref="AF39:AF41" si="8">ROUND(P29,2)&amp;"%"</f>
+        <v>0,91%</v>
+      </c>
+    </row>
+    <row r="40" spans="9:32" x14ac:dyDescent="0.35">
       <c r="I40" t="s">
         <v>612</v>
       </c>
-      <c r="K40" s="13">
+      <c r="K40" s="12">
         <v>3.8589190000000002</v>
       </c>
-      <c r="L40" s="13">
+      <c r="L40" s="12">
         <v>5.7759210000000003</v>
       </c>
-      <c r="M40" s="13">
+      <c r="M40" s="12">
         <v>2.9577749999999998</v>
       </c>
-      <c r="N40" s="13">
+      <c r="N40" s="12">
         <v>4.1816709999999997</v>
       </c>
-      <c r="O40" s="13">
+      <c r="O40" s="12">
         <v>2.9247450000000002</v>
       </c>
-      <c r="P40" s="13">
+      <c r="P40" s="12">
         <v>4.1689720000000001</v>
       </c>
-    </row>
-    <row r="41" spans="9:17" x14ac:dyDescent="0.35">
+      <c r="X40" t="s">
+        <v>623</v>
+      </c>
+      <c r="Y40" s="25">
+        <v>0.58889384258172439</v>
+      </c>
+      <c r="Z40" s="27" t="str">
+        <f t="shared" si="5"/>
+        <v>3,39%</v>
+      </c>
+      <c r="AA40" s="25">
+        <v>0.69002561197986123</v>
+      </c>
+      <c r="AB40" s="27" t="str">
+        <f t="shared" si="6"/>
+        <v>4,34%</v>
+      </c>
+      <c r="AC40" s="25">
+        <v>0.7317529997594584</v>
+      </c>
+      <c r="AD40" s="27" t="str">
+        <f t="shared" si="7"/>
+        <v>0,81%</v>
+      </c>
+      <c r="AE40" s="25">
+        <v>0.64485639706193698</v>
+      </c>
+      <c r="AF40" s="27" t="str">
+        <f t="shared" si="8"/>
+        <v>1,08%</v>
+      </c>
+    </row>
+    <row r="41" spans="9:32" x14ac:dyDescent="0.35">
       <c r="I41" t="s">
         <v>613</v>
       </c>
-      <c r="K41" s="13">
+      <c r="K41" s="12">
         <v>3.8382070000000001</v>
       </c>
-      <c r="L41" s="13">
+      <c r="L41" s="12">
         <v>5.5115879999999997</v>
       </c>
-      <c r="M41" s="13">
+      <c r="M41" s="12">
         <v>2.981779</v>
       </c>
-      <c r="N41" s="13">
+      <c r="N41" s="12">
         <v>4.1152639999999998</v>
       </c>
-      <c r="O41" s="13">
+      <c r="O41" s="12">
         <v>2.9371160000000001</v>
       </c>
-      <c r="P41" s="13">
+      <c r="P41" s="12">
         <v>4.1176490000000001</v>
       </c>
+      <c r="X41" t="s">
+        <v>624</v>
+      </c>
+      <c r="Y41" s="25">
+        <v>0</v>
+      </c>
+      <c r="Z41" s="27" t="str">
+        <f t="shared" si="5"/>
+        <v>3,33%</v>
+      </c>
+      <c r="AA41" s="25">
+        <v>0</v>
+      </c>
+      <c r="AB41" s="27" t="str">
+        <f t="shared" si="6"/>
+        <v>4,1%</v>
+      </c>
+      <c r="AC41" s="25">
+        <v>0.72042543081963584</v>
+      </c>
+      <c r="AD41" s="27" t="str">
+        <f t="shared" si="7"/>
+        <v>0,73%</v>
+      </c>
+      <c r="AE41" s="25">
+        <v>0.55779226413010896</v>
+      </c>
+      <c r="AF41" s="27" t="str">
+        <f t="shared" si="8"/>
+        <v>0,85%</v>
+      </c>
+    </row>
+    <row r="45" spans="9:32" x14ac:dyDescent="0.35">
+      <c r="X45" s="30"/>
+      <c r="Y45">
+        <v>1</v>
+      </c>
+      <c r="Z45">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="46" spans="9:32" x14ac:dyDescent="0.35">
+      <c r="X46" s="30" t="s">
+        <v>622</v>
+      </c>
+      <c r="Y46" t="s">
+        <v>636</v>
+      </c>
+      <c r="Z46" t="s">
+        <v>637</v>
+      </c>
+    </row>
+    <row r="47" spans="9:32" x14ac:dyDescent="0.35">
+      <c r="X47" s="30" t="s">
+        <v>623</v>
+      </c>
+      <c r="Y47" t="s">
+        <v>638</v>
+      </c>
+      <c r="Z47" t="s">
+        <v>639</v>
+      </c>
+    </row>
+    <row r="48" spans="9:32" x14ac:dyDescent="0.35">
+      <c r="X48" s="31" t="s">
+        <v>624</v>
+      </c>
+      <c r="Y48" t="s">
+        <v>640</v>
+      </c>
+      <c r="Z48" t="s">
+        <v>641</v>
+      </c>
     </row>
   </sheetData>
+  <mergeCells count="6">
+    <mergeCell ref="Y35:AB35"/>
+    <mergeCell ref="AC35:AF35"/>
+    <mergeCell ref="Y36:Z36"/>
+    <mergeCell ref="AA36:AB36"/>
+    <mergeCell ref="AC36:AD36"/>
+    <mergeCell ref="AE36:AF36"/>
+  </mergeCells>
   <phoneticPr fontId="8" type="noConversion"/>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
 </worksheet>

</xml_diff>

<commit_message>
Organized code for main and main_ibc, generated graphs with results
</commit_message>
<xml_diff>
--- a/Data Info/DadosEscolhidos.xlsx
+++ b/Data Info/DadosEscolhidos.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/ad5e0ae908eb1af8/Documentos/GitHub/gdp-forecasting-with-ML/Data Info/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="2401" documentId="11_AD4D361C20488DEA4E38A0E30418638E5BDEDD8E" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{9BE02FB7-C322-49F9-A54B-FB93B901241F}"/>
+  <xr:revisionPtr revIDLastSave="2552" documentId="11_AD4D361C20488DEA4E38A0E30418638E5BDEDD8E" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{DDF44AD6-27A0-4765-AB12-E367BA1FBCF2}"/>
   <bookViews>
-    <workbookView xWindow="-45" yWindow="-16320" windowWidth="29040" windowHeight="15720" firstSheet="2" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Official Series - Quarterly" sheetId="7" r:id="rId1"/>
@@ -19,8 +19,9 @@
     <sheet name="Table M" sheetId="10" r:id="rId4"/>
     <sheet name="All Series" sheetId="1" state="hidden" r:id="rId5"/>
     <sheet name="All Series (2)" sheetId="6" state="hidden" r:id="rId6"/>
-    <sheet name="Planilha1" sheetId="11" r:id="rId7"/>
-    <sheet name="exports_SAseries" sheetId="3" state="hidden" r:id="rId8"/>
+    <sheet name="Results" sheetId="12" r:id="rId7"/>
+    <sheet name="Results - test" sheetId="11" r:id="rId8"/>
+    <sheet name="exports_SAseries" sheetId="3" state="hidden" r:id="rId9"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Official Series - Quarterly'!$A$1:$J$101</definedName>
@@ -46,7 +47,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6358" uniqueCount="642">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6471" uniqueCount="659">
   <si>
     <t>NSAprod_cam_br</t>
   </si>
@@ -2009,6 +2010,57 @@
   <si>
     <t>"2.155552e-07***"</t>
   </si>
+  <si>
+    <t>"0.0218072228*"</t>
+  </si>
+  <si>
+    <t>"0.2291410844"</t>
+  </si>
+  <si>
+    <t>"0.0281022508*"</t>
+  </si>
+  <si>
+    <t>"0.2185918042"</t>
+  </si>
+  <si>
+    <t>"0.0063982168**"</t>
+  </si>
+  <si>
+    <t>"0.1579516395"</t>
+  </si>
+  <si>
+    <t>benchmarkq</t>
+  </si>
+  <si>
+    <t>lasso_modelq</t>
+  </si>
+  <si>
+    <t>enet_modelq</t>
+  </si>
+  <si>
+    <t>rf_modelq</t>
+  </si>
+  <si>
+    <t>Diebold-Mariano</t>
+  </si>
+  <si>
+    <t>monthly</t>
+  </si>
+  <si>
+    <t xml:space="preserve">h = 1 </t>
+  </si>
+  <si>
+    <t>h = 12</t>
+  </si>
+  <si>
+    <t>h = 4</t>
+  </si>
+  <si>
+    <t>Horizon</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MAPE (%) </t>
+  </si>
 </sst>
 </file>
 
@@ -2017,10 +2069,10 @@
   <numFmts count="4">
     <numFmt numFmtId="164" formatCode="#,##0.0000"/>
     <numFmt numFmtId="165" formatCode="0.0000"/>
-    <numFmt numFmtId="167" formatCode="0.000"/>
-    <numFmt numFmtId="174" formatCode="#,##0.000"/>
+    <numFmt numFmtId="166" formatCode="0.000"/>
+    <numFmt numFmtId="167" formatCode="#,##0.000"/>
   </numFmts>
-  <fonts count="9" x14ac:knownFonts="1">
+  <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -2080,8 +2132,15 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="7"/>
+      <color rgb="FF4D4D4C"/>
+      <name val="Cascadia Code"/>
+      <family val="3"/>
+    </font>
   </fonts>
-  <fills count="8">
+  <fills count="9">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -2124,8 +2183,14 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -2142,13 +2207,22 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="32">
+  <cellXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -2208,20 +2282,65 @@
     <xf numFmtId="165" fontId="7" fillId="7" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="4" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="4" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="174" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="4" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="4" fontId="7" fillId="8" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="7" fillId="8" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="7" fillId="8" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="167" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="166" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="4" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="4" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="4" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="4" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="4" fontId="6" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -23627,11 +23746,913 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{540FB65C-DB34-4596-B31F-FC859CCB543C}">
+  <dimension ref="B2:R40"/>
+  <sheetViews>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A17" zoomScale="105" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="L29" sqref="L29"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="2" max="2" width="13.7265625" customWidth="1"/>
+    <col min="4" max="4" width="8.7265625" customWidth="1"/>
+    <col min="5" max="5" width="0.453125" customWidth="1"/>
+    <col min="8" max="8" width="8.7265625" customWidth="1"/>
+    <col min="11" max="11" width="8.81640625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="9.54296875" bestFit="1" customWidth="1"/>
+    <col min="13" max="15" width="8.81640625" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="10.08984375" bestFit="1" customWidth="1"/>
+    <col min="17" max="18" width="16.7265625" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="13" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="2:18" x14ac:dyDescent="0.35">
+      <c r="D2" t="s">
+        <v>654</v>
+      </c>
+      <c r="E2" t="s">
+        <v>654</v>
+      </c>
+      <c r="F2" t="s">
+        <v>654</v>
+      </c>
+      <c r="G2" t="s">
+        <v>656</v>
+      </c>
+      <c r="H2" t="s">
+        <v>656</v>
+      </c>
+      <c r="I2" t="s">
+        <v>656</v>
+      </c>
+      <c r="P2" t="s">
+        <v>652</v>
+      </c>
+    </row>
+    <row r="3" spans="2:18" x14ac:dyDescent="0.35">
+      <c r="D3" t="s">
+        <v>578</v>
+      </c>
+      <c r="E3" t="s">
+        <v>579</v>
+      </c>
+      <c r="F3" t="s">
+        <v>580</v>
+      </c>
+      <c r="G3" t="s">
+        <v>578</v>
+      </c>
+      <c r="H3" t="s">
+        <v>579</v>
+      </c>
+      <c r="I3" t="s">
+        <v>580</v>
+      </c>
+    </row>
+    <row r="4" spans="2:18" x14ac:dyDescent="0.35">
+      <c r="B4" s="10" t="s">
+        <v>648</v>
+      </c>
+      <c r="C4" s="10"/>
+      <c r="D4" s="14">
+        <v>10.138339999999999</v>
+      </c>
+      <c r="E4" s="14">
+        <v>7.387079</v>
+      </c>
+      <c r="F4" s="14">
+        <v>5.4638929999999997</v>
+      </c>
+      <c r="G4" s="14">
+        <v>11.06123</v>
+      </c>
+      <c r="H4" s="14">
+        <v>7.043361</v>
+      </c>
+      <c r="I4" s="14">
+        <v>5.0934699999999999</v>
+      </c>
+      <c r="J4" t="s">
+        <v>595</v>
+      </c>
+      <c r="P4" s="38" t="s">
+        <v>653</v>
+      </c>
+      <c r="Q4">
+        <v>1</v>
+      </c>
+      <c r="R4">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="5" spans="2:18" x14ac:dyDescent="0.35">
+      <c r="B5" t="s">
+        <v>649</v>
+      </c>
+      <c r="D5" s="32">
+        <v>5.3612840000000004</v>
+      </c>
+      <c r="E5" s="32">
+        <v>4.273517</v>
+      </c>
+      <c r="F5" s="32">
+        <v>3.1899090000000001</v>
+      </c>
+      <c r="G5" s="31">
+        <v>7.6462380000000003</v>
+      </c>
+      <c r="H5" s="31">
+        <v>5.8681039999999998</v>
+      </c>
+      <c r="I5" s="31">
+        <v>4.3203310000000004</v>
+      </c>
+      <c r="P5" s="28" t="s">
+        <v>622</v>
+      </c>
+      <c r="Q5" t="s">
+        <v>636</v>
+      </c>
+      <c r="R5" t="s">
+        <v>637</v>
+      </c>
+    </row>
+    <row r="6" spans="2:18" x14ac:dyDescent="0.35">
+      <c r="B6" t="s">
+        <v>650</v>
+      </c>
+      <c r="D6" s="31">
+        <v>5.9704059999999997</v>
+      </c>
+      <c r="E6" s="31">
+        <v>4.5451629999999996</v>
+      </c>
+      <c r="F6" s="31">
+        <v>3.3889990000000001</v>
+      </c>
+      <c r="G6" s="31">
+        <v>7.6325320000000003</v>
+      </c>
+      <c r="H6" s="31">
+        <v>5.8982469999999996</v>
+      </c>
+      <c r="I6" s="31">
+        <v>4.3434660000000003</v>
+      </c>
+      <c r="P6" s="28" t="s">
+        <v>623</v>
+      </c>
+      <c r="Q6" t="s">
+        <v>638</v>
+      </c>
+      <c r="R6" t="s">
+        <v>639</v>
+      </c>
+    </row>
+    <row r="7" spans="2:18" x14ac:dyDescent="0.35">
+      <c r="B7" t="s">
+        <v>651</v>
+      </c>
+      <c r="D7" s="11">
+        <v>7.4797289999999998</v>
+      </c>
+      <c r="E7" s="11">
+        <v>4.6017210000000004</v>
+      </c>
+      <c r="F7" s="11">
+        <v>3.3251400000000002</v>
+      </c>
+      <c r="G7" s="32">
+        <v>7.5066800000000002</v>
+      </c>
+      <c r="H7" s="32">
+        <v>5.5938590000000001</v>
+      </c>
+      <c r="I7" s="32">
+        <v>4.095269</v>
+      </c>
+      <c r="P7" s="29" t="s">
+        <v>624</v>
+      </c>
+      <c r="Q7" t="s">
+        <v>640</v>
+      </c>
+      <c r="R7" t="s">
+        <v>641</v>
+      </c>
+    </row>
+    <row r="9" spans="2:18" x14ac:dyDescent="0.35">
+      <c r="D9" t="s">
+        <v>578</v>
+      </c>
+      <c r="E9" t="s">
+        <v>579</v>
+      </c>
+      <c r="F9" t="s">
+        <v>580</v>
+      </c>
+      <c r="G9" t="s">
+        <v>578</v>
+      </c>
+      <c r="H9" t="s">
+        <v>579</v>
+      </c>
+      <c r="I9" t="s">
+        <v>580</v>
+      </c>
+      <c r="P9" s="38" t="s">
+        <v>529</v>
+      </c>
+      <c r="Q9">
+        <v>1</v>
+      </c>
+      <c r="R9">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="10" spans="2:18" x14ac:dyDescent="0.35">
+      <c r="D10" t="s">
+        <v>654</v>
+      </c>
+      <c r="E10" t="s">
+        <v>654</v>
+      </c>
+      <c r="F10" t="s">
+        <v>654</v>
+      </c>
+      <c r="G10" t="s">
+        <v>655</v>
+      </c>
+      <c r="H10" t="s">
+        <v>655</v>
+      </c>
+      <c r="I10" t="s">
+        <v>655</v>
+      </c>
+      <c r="P10" s="28" t="s">
+        <v>622</v>
+      </c>
+      <c r="Q10" t="s">
+        <v>642</v>
+      </c>
+      <c r="R10" t="s">
+        <v>643</v>
+      </c>
+    </row>
+    <row r="11" spans="2:18" x14ac:dyDescent="0.35">
+      <c r="B11" t="s">
+        <v>615</v>
+      </c>
+      <c r="D11" s="33">
+        <v>6.7389569999999996E-2</v>
+      </c>
+      <c r="E11" s="33">
+        <v>5.007342E-2</v>
+      </c>
+      <c r="F11" s="33">
+        <v>1.0766389999999999</v>
+      </c>
+      <c r="G11" s="33">
+        <v>9.6357360000000003E-2</v>
+      </c>
+      <c r="H11" s="33">
+        <v>6.8928249999999996E-2</v>
+      </c>
+      <c r="I11" s="33">
+        <v>1.4784839999999999</v>
+      </c>
+      <c r="J11" t="s">
+        <v>598</v>
+      </c>
+      <c r="P11" s="28" t="s">
+        <v>623</v>
+      </c>
+      <c r="Q11" t="s">
+        <v>644</v>
+      </c>
+      <c r="R11" t="s">
+        <v>645</v>
+      </c>
+    </row>
+    <row r="12" spans="2:18" x14ac:dyDescent="0.35">
+      <c r="B12" t="s">
+        <v>616</v>
+      </c>
+      <c r="D12" s="36">
+        <v>3.5456799999999997E-2</v>
+      </c>
+      <c r="E12" s="36">
+        <v>2.732362E-2</v>
+      </c>
+      <c r="F12" s="36">
+        <v>0.59215430000000002</v>
+      </c>
+      <c r="G12" s="34">
+        <v>5.7688940000000001E-2</v>
+      </c>
+      <c r="H12" s="34">
+        <v>4.1704409999999997E-2</v>
+      </c>
+      <c r="I12" s="34">
+        <v>0.90730739999999999</v>
+      </c>
+      <c r="P12" s="29" t="s">
+        <v>624</v>
+      </c>
+      <c r="Q12" t="s">
+        <v>646</v>
+      </c>
+      <c r="R12" t="s">
+        <v>647</v>
+      </c>
+    </row>
+    <row r="13" spans="2:18" x14ac:dyDescent="0.35">
+      <c r="B13" t="s">
+        <v>617</v>
+      </c>
+      <c r="D13" s="34">
+        <v>4.9312519999999999E-2</v>
+      </c>
+      <c r="E13" s="34">
+        <v>3.7580210000000003E-2</v>
+      </c>
+      <c r="F13" s="34">
+        <v>0.81035729999999995</v>
+      </c>
+      <c r="G13" s="34">
+        <v>6.2136660000000003E-2</v>
+      </c>
+      <c r="H13" s="34">
+        <v>4.9575040000000001E-2</v>
+      </c>
+      <c r="I13" s="34">
+        <v>1.0750708</v>
+      </c>
+    </row>
+    <row r="14" spans="2:18" x14ac:dyDescent="0.35">
+      <c r="B14" t="s">
+        <v>618</v>
+      </c>
+      <c r="D14" s="35">
+        <v>4.8549160000000001E-2</v>
+      </c>
+      <c r="E14" s="35">
+        <v>3.3600360000000003E-2</v>
+      </c>
+      <c r="F14" s="35">
+        <v>0.72549490000000005</v>
+      </c>
+      <c r="G14" s="37">
+        <v>5.3747389999999999E-2</v>
+      </c>
+      <c r="H14" s="37">
+        <v>3.9196839999999997E-2</v>
+      </c>
+      <c r="I14" s="37">
+        <v>0.84613229999999995</v>
+      </c>
+    </row>
+    <row r="17" spans="2:13" x14ac:dyDescent="0.35">
+      <c r="B17" t="s">
+        <v>633</v>
+      </c>
+    </row>
+    <row r="19" spans="2:13" x14ac:dyDescent="0.35">
+      <c r="B19" s="45" t="s">
+        <v>658</v>
+      </c>
+      <c r="C19" s="48" t="s">
+        <v>627</v>
+      </c>
+      <c r="D19" s="48"/>
+      <c r="F19" s="48" t="s">
+        <v>626</v>
+      </c>
+      <c r="G19" s="48"/>
+      <c r="I19" t="s">
+        <v>625</v>
+      </c>
+      <c r="J19" t="s">
+        <v>627</v>
+      </c>
+      <c r="L19" t="s">
+        <v>626</v>
+      </c>
+    </row>
+    <row r="20" spans="2:13" x14ac:dyDescent="0.35">
+      <c r="B20" t="s">
+        <v>657</v>
+      </c>
+      <c r="C20">
+        <v>1</v>
+      </c>
+      <c r="D20" s="45">
+        <v>12</v>
+      </c>
+      <c r="E20" s="45"/>
+      <c r="F20" s="45">
+        <v>1</v>
+      </c>
+      <c r="G20" s="45">
+        <v>4</v>
+      </c>
+      <c r="J20" t="s">
+        <v>628</v>
+      </c>
+      <c r="K20" t="s">
+        <v>630</v>
+      </c>
+      <c r="L20" t="s">
+        <v>628</v>
+      </c>
+      <c r="M20" t="s">
+        <v>629</v>
+      </c>
+    </row>
+    <row r="21" spans="2:13" x14ac:dyDescent="0.35">
+      <c r="B21" s="10" t="s">
+        <v>631</v>
+      </c>
+      <c r="C21" s="41">
+        <f>ROUND(F11,2)</f>
+        <v>1.08</v>
+      </c>
+      <c r="D21" s="44" t="str">
+        <f>ROUND(I11,2)&amp;"%"</f>
+        <v>1,48%</v>
+      </c>
+      <c r="F21" s="44" t="str">
+        <f>ROUND(F4,2)&amp;"%"</f>
+        <v>5,46%</v>
+      </c>
+      <c r="G21" s="44" t="str">
+        <f>ROUND(I4,2)&amp;"%"</f>
+        <v>5,09%</v>
+      </c>
+      <c r="I21" t="s">
+        <v>631</v>
+      </c>
+      <c r="J21" s="25">
+        <v>1</v>
+      </c>
+      <c r="K21" s="25">
+        <v>1</v>
+      </c>
+      <c r="L21" s="25">
+        <v>1</v>
+      </c>
+      <c r="M21" s="25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="22" spans="2:13" x14ac:dyDescent="0.35">
+      <c r="B22" s="42" t="s">
+        <v>622</v>
+      </c>
+      <c r="C22" s="43">
+        <f>ROUND(F12,2)</f>
+        <v>0.59</v>
+      </c>
+      <c r="D22" s="44" t="str">
+        <f>ROUND(I12,2)&amp;"%"</f>
+        <v>0,91%</v>
+      </c>
+      <c r="F22" s="43" t="str">
+        <f>ROUND(F5,2)&amp;"%"</f>
+        <v>3,19%</v>
+      </c>
+      <c r="G22" s="44" t="str">
+        <f>ROUND(I5,2)&amp;"%"</f>
+        <v>4,32%</v>
+      </c>
+      <c r="I22" t="s">
+        <v>622</v>
+      </c>
+      <c r="J22" s="40">
+        <f>D12/$D$11</f>
+        <v>0.5261467019302839</v>
+      </c>
+      <c r="K22" s="25">
+        <f>G12/$G$11</f>
+        <v>0.59869780575142362</v>
+      </c>
+      <c r="L22" s="40">
+        <f>D5/$D$4</f>
+        <v>0.52881280367397432</v>
+      </c>
+      <c r="M22" s="25">
+        <f>G5/$G$4</f>
+        <v>0.69126471468362927</v>
+      </c>
+    </row>
+    <row r="23" spans="2:13" x14ac:dyDescent="0.35">
+      <c r="B23" s="42" t="s">
+        <v>623</v>
+      </c>
+      <c r="C23" s="44">
+        <f>ROUND(F13,2)</f>
+        <v>0.81</v>
+      </c>
+      <c r="D23" s="44" t="str">
+        <f>ROUND(I13,2)&amp;"%"</f>
+        <v>1,08%</v>
+      </c>
+      <c r="F23" s="44" t="str">
+        <f>ROUND(F6,2)&amp;"%"</f>
+        <v>3,39%</v>
+      </c>
+      <c r="G23" s="44" t="str">
+        <f>ROUND(I6,2)&amp;"%"</f>
+        <v>4,34%</v>
+      </c>
+      <c r="I23" t="s">
+        <v>623</v>
+      </c>
+      <c r="J23" s="25">
+        <f>D13/$D$11</f>
+        <v>0.7317529997594584</v>
+      </c>
+      <c r="K23" s="25">
+        <f>G13/$G$11</f>
+        <v>0.64485639706193698</v>
+      </c>
+      <c r="L23" s="25">
+        <f>D6/$D$4</f>
+        <v>0.58889384258172439</v>
+      </c>
+      <c r="M23" s="25">
+        <f>G6/$G$4</f>
+        <v>0.69002561197986123</v>
+      </c>
+    </row>
+    <row r="24" spans="2:13" x14ac:dyDescent="0.35">
+      <c r="B24" s="45" t="s">
+        <v>624</v>
+      </c>
+      <c r="C24" s="46" t="str">
+        <f>ROUND(F14,2)&amp;"%"</f>
+        <v>0,73%</v>
+      </c>
+      <c r="D24" s="47" t="str">
+        <f>ROUND(I14,2)&amp;"%"</f>
+        <v>0,85%</v>
+      </c>
+      <c r="E24" s="45"/>
+      <c r="F24" s="46" t="str">
+        <f>ROUND(F7,2)&amp;"%"</f>
+        <v>3,33%</v>
+      </c>
+      <c r="G24" s="47" t="str">
+        <f>ROUND(I7,2)&amp;"%"</f>
+        <v>4,1%</v>
+      </c>
+      <c r="I24" t="s">
+        <v>624</v>
+      </c>
+      <c r="J24" s="25">
+        <f>D14/$D$11</f>
+        <v>0.72042543081963584</v>
+      </c>
+      <c r="K24" s="40">
+        <f>G14/$G$11</f>
+        <v>0.55779226413010896</v>
+      </c>
+      <c r="L24" s="25">
+        <f>D7/$D$4</f>
+        <v>0.73776663635269679</v>
+      </c>
+      <c r="M24" s="40">
+        <f>G7/$G$4</f>
+        <v>0.67864785381010972</v>
+      </c>
+    </row>
+    <row r="26" spans="2:13" x14ac:dyDescent="0.35">
+      <c r="C26" s="30" t="s">
+        <v>627</v>
+      </c>
+      <c r="D26" s="30"/>
+      <c r="F26" s="30" t="s">
+        <v>626</v>
+      </c>
+      <c r="G26" s="30"/>
+    </row>
+    <row r="27" spans="2:13" x14ac:dyDescent="0.35">
+      <c r="C27" t="s">
+        <v>628</v>
+      </c>
+      <c r="D27" t="s">
+        <v>630</v>
+      </c>
+      <c r="F27" t="s">
+        <v>628</v>
+      </c>
+      <c r="G27" t="s">
+        <v>629</v>
+      </c>
+    </row>
+    <row r="28" spans="2:13" x14ac:dyDescent="0.35">
+      <c r="B28" t="s">
+        <v>631</v>
+      </c>
+      <c r="C28" s="27">
+        <f>D11</f>
+        <v>6.7389569999999996E-2</v>
+      </c>
+      <c r="D28" s="27">
+        <f>G11</f>
+        <v>9.6357360000000003E-2</v>
+      </c>
+      <c r="F28" s="27">
+        <f>D4</f>
+        <v>10.138339999999999</v>
+      </c>
+      <c r="G28" s="27">
+        <f>G4</f>
+        <v>11.06123</v>
+      </c>
+    </row>
+    <row r="29" spans="2:13" x14ac:dyDescent="0.35">
+      <c r="B29" t="s">
+        <v>622</v>
+      </c>
+      <c r="C29" s="39">
+        <f>D12</f>
+        <v>3.5456799999999997E-2</v>
+      </c>
+      <c r="D29" s="27">
+        <f>G12</f>
+        <v>5.7688940000000001E-2</v>
+      </c>
+      <c r="F29" s="39">
+        <f>D5</f>
+        <v>5.3612840000000004</v>
+      </c>
+      <c r="G29" s="27">
+        <f>G5</f>
+        <v>7.6462380000000003</v>
+      </c>
+    </row>
+    <row r="30" spans="2:13" x14ac:dyDescent="0.35">
+      <c r="B30" t="s">
+        <v>623</v>
+      </c>
+      <c r="C30" s="27">
+        <f>D13</f>
+        <v>4.9312519999999999E-2</v>
+      </c>
+      <c r="D30" s="27">
+        <f>G13</f>
+        <v>6.2136660000000003E-2</v>
+      </c>
+      <c r="F30" s="27">
+        <f>D6</f>
+        <v>5.9704059999999997</v>
+      </c>
+      <c r="G30" s="27">
+        <f>G6</f>
+        <v>7.6325320000000003</v>
+      </c>
+    </row>
+    <row r="31" spans="2:13" x14ac:dyDescent="0.35">
+      <c r="B31" t="s">
+        <v>624</v>
+      </c>
+      <c r="C31" s="27">
+        <f>D14</f>
+        <v>4.8549160000000001E-2</v>
+      </c>
+      <c r="D31" s="39">
+        <f>G14</f>
+        <v>5.3747389999999999E-2</v>
+      </c>
+      <c r="F31" s="27">
+        <f>D7</f>
+        <v>7.4797289999999998</v>
+      </c>
+      <c r="G31" s="39">
+        <f>G7</f>
+        <v>7.5066800000000002</v>
+      </c>
+    </row>
+    <row r="33" spans="2:10" x14ac:dyDescent="0.35">
+      <c r="B33" t="s">
+        <v>634</v>
+      </c>
+    </row>
+    <row r="34" spans="2:10" x14ac:dyDescent="0.35">
+      <c r="C34" s="30" t="s">
+        <v>626</v>
+      </c>
+      <c r="D34" s="30"/>
+      <c r="E34" s="30"/>
+      <c r="F34" s="30"/>
+      <c r="G34" s="30" t="s">
+        <v>627</v>
+      </c>
+      <c r="H34" s="30"/>
+      <c r="I34" s="30"/>
+      <c r="J34" s="30"/>
+    </row>
+    <row r="35" spans="2:10" x14ac:dyDescent="0.35">
+      <c r="C35" s="30" t="s">
+        <v>628</v>
+      </c>
+      <c r="D35" s="30"/>
+      <c r="E35" s="30" t="s">
+        <v>629</v>
+      </c>
+      <c r="F35" s="30"/>
+      <c r="G35" s="30" t="s">
+        <v>628</v>
+      </c>
+      <c r="H35" s="30"/>
+      <c r="I35" s="30" t="s">
+        <v>630</v>
+      </c>
+      <c r="J35" s="30"/>
+    </row>
+    <row r="36" spans="2:10" x14ac:dyDescent="0.35">
+      <c r="C36" t="s">
+        <v>625</v>
+      </c>
+      <c r="D36" t="s">
+        <v>580</v>
+      </c>
+      <c r="E36" t="s">
+        <v>625</v>
+      </c>
+      <c r="F36" t="s">
+        <v>580</v>
+      </c>
+      <c r="G36" t="s">
+        <v>625</v>
+      </c>
+      <c r="H36" t="s">
+        <v>580</v>
+      </c>
+      <c r="I36" t="s">
+        <v>625</v>
+      </c>
+      <c r="J36" t="s">
+        <v>580</v>
+      </c>
+    </row>
+    <row r="37" spans="2:10" x14ac:dyDescent="0.35">
+      <c r="B37" t="s">
+        <v>631</v>
+      </c>
+      <c r="C37" s="25">
+        <v>1</v>
+      </c>
+      <c r="D37" s="26" t="str">
+        <f>ROUND(F4,2)&amp;"%"</f>
+        <v>5,46%</v>
+      </c>
+      <c r="E37" s="25">
+        <v>1</v>
+      </c>
+      <c r="F37" s="26" t="str">
+        <f>ROUND(I4,2)&amp;"%"</f>
+        <v>5,09%</v>
+      </c>
+      <c r="G37" s="25">
+        <v>1</v>
+      </c>
+      <c r="H37" s="26" t="str">
+        <f>ROUND(F11,2)&amp;"%"</f>
+        <v>1,08%</v>
+      </c>
+      <c r="I37" s="25">
+        <v>1</v>
+      </c>
+      <c r="J37" s="26" t="str">
+        <f>ROUND(I11,2)&amp;"%"</f>
+        <v>1,48%</v>
+      </c>
+    </row>
+    <row r="38" spans="2:10" x14ac:dyDescent="0.35">
+      <c r="B38" t="s">
+        <v>622</v>
+      </c>
+      <c r="C38" s="25">
+        <v>0.52881280367397432</v>
+      </c>
+      <c r="D38" s="26" t="str">
+        <f>ROUND(F5,2)&amp;"%"</f>
+        <v>3,19%</v>
+      </c>
+      <c r="E38" s="25">
+        <v>0.69126471468362927</v>
+      </c>
+      <c r="F38" s="26" t="str">
+        <f>ROUND(I5,2)&amp;"%"</f>
+        <v>4,32%</v>
+      </c>
+      <c r="G38" s="25">
+        <v>0.5261467019302839</v>
+      </c>
+      <c r="H38" s="26" t="str">
+        <f>ROUND(F12,2)&amp;"%"</f>
+        <v>0,59%</v>
+      </c>
+      <c r="I38" s="25">
+        <v>0.59869780575142362</v>
+      </c>
+      <c r="J38" s="26" t="str">
+        <f>ROUND(I12,2)&amp;"%"</f>
+        <v>0,91%</v>
+      </c>
+    </row>
+    <row r="39" spans="2:10" x14ac:dyDescent="0.35">
+      <c r="B39" t="s">
+        <v>623</v>
+      </c>
+      <c r="C39" s="25">
+        <v>0.58889384258172439</v>
+      </c>
+      <c r="D39" s="26" t="str">
+        <f>ROUND(F6,2)&amp;"%"</f>
+        <v>3,39%</v>
+      </c>
+      <c r="E39" s="25">
+        <v>0.69002561197986123</v>
+      </c>
+      <c r="F39" s="26" t="str">
+        <f>ROUND(I6,2)&amp;"%"</f>
+        <v>4,34%</v>
+      </c>
+      <c r="G39" s="25">
+        <v>0.7317529997594584</v>
+      </c>
+      <c r="H39" s="26" t="str">
+        <f>ROUND(F13,2)&amp;"%"</f>
+        <v>0,81%</v>
+      </c>
+      <c r="I39" s="25">
+        <v>0.64485639706193698</v>
+      </c>
+      <c r="J39" s="26" t="str">
+        <f>ROUND(I13,2)&amp;"%"</f>
+        <v>1,08%</v>
+      </c>
+    </row>
+    <row r="40" spans="2:10" x14ac:dyDescent="0.35">
+      <c r="B40" t="s">
+        <v>624</v>
+      </c>
+      <c r="C40" s="25">
+        <v>0</v>
+      </c>
+      <c r="D40" s="26" t="str">
+        <f>ROUND(F7,2)&amp;"%"</f>
+        <v>3,33%</v>
+      </c>
+      <c r="E40" s="25">
+        <v>0</v>
+      </c>
+      <c r="F40" s="26" t="str">
+        <f>ROUND(I7,2)&amp;"%"</f>
+        <v>4,1%</v>
+      </c>
+      <c r="G40" s="25">
+        <v>0.72042543081963584</v>
+      </c>
+      <c r="H40" s="26" t="str">
+        <f>ROUND(F14,2)&amp;"%"</f>
+        <v>0,73%</v>
+      </c>
+      <c r="I40" s="25">
+        <v>0.55779226413010896</v>
+      </c>
+      <c r="J40" s="26" t="str">
+        <f>ROUND(I14,2)&amp;"%"</f>
+        <v>0,85%</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="10">
+    <mergeCell ref="C19:D19"/>
+    <mergeCell ref="F19:G19"/>
+    <mergeCell ref="C26:D26"/>
+    <mergeCell ref="F26:G26"/>
+    <mergeCell ref="C34:F34"/>
+    <mergeCell ref="G34:J34"/>
+    <mergeCell ref="C35:D35"/>
+    <mergeCell ref="E35:F35"/>
+    <mergeCell ref="G35:H35"/>
+    <mergeCell ref="I35:J35"/>
+  </mergeCells>
+  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3870FAA5-0C9A-4077-820D-651F982FFC52}">
-  <dimension ref="H3:AI48"/>
+  <dimension ref="H3:AI53"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="105" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="Q20" sqref="Q20"/>
+    <sheetView zoomScale="105" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="M14" sqref="M14:N14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -23917,8 +24938,12 @@
       <c r="L14" s="11">
         <v>7.5066800000000002</v>
       </c>
-      <c r="M14" s="26"/>
-      <c r="N14" s="26"/>
+      <c r="M14" s="11">
+        <v>4.6017210000000004</v>
+      </c>
+      <c r="N14" s="11">
+        <v>5.5938590000000001</v>
+      </c>
       <c r="O14" s="11">
         <v>3.3251400000000002</v>
       </c>
@@ -24120,20 +25145,20 @@
       <c r="X22" t="s">
         <v>631</v>
       </c>
-      <c r="Y22" s="27" t="str">
-        <f>ROUND(O11,2)&amp;"%"</f>
+      <c r="Y22" s="26" t="str">
+        <f t="shared" ref="Y22:Z25" si="0">ROUND(O11,2)&amp;"%"</f>
         <v>5,46%</v>
       </c>
-      <c r="Z22" s="27" t="str">
-        <f>ROUND(P11,2)&amp;"%"</f>
+      <c r="Z22" s="26" t="str">
+        <f t="shared" si="0"/>
         <v>5,09%</v>
       </c>
-      <c r="AA22" s="27" t="str">
-        <f>ROUND(O28,2)&amp;"%"</f>
+      <c r="AA22" s="26" t="str">
+        <f t="shared" ref="AA22:AB25" si="1">ROUND(O28,2)&amp;"%"</f>
         <v>1,08%</v>
       </c>
-      <c r="AB22" s="27" t="str">
-        <f>ROUND(P28,2)&amp;"%"</f>
+      <c r="AB22" s="26" t="str">
+        <f t="shared" si="1"/>
         <v>1,48%</v>
       </c>
     </row>
@@ -24159,20 +25184,20 @@
       <c r="X23" t="s">
         <v>622</v>
       </c>
-      <c r="Y23" s="27" t="str">
-        <f>ROUND(O12,2)&amp;"%"</f>
+      <c r="Y23" s="26" t="str">
+        <f t="shared" si="0"/>
         <v>3,19%</v>
       </c>
-      <c r="Z23" s="27" t="str">
-        <f>ROUND(P12,2)&amp;"%"</f>
+      <c r="Z23" s="26" t="str">
+        <f t="shared" si="0"/>
         <v>4,32%</v>
       </c>
-      <c r="AA23" s="27" t="str">
-        <f>ROUND(O29,2)&amp;"%"</f>
+      <c r="AA23" s="26" t="str">
+        <f t="shared" si="1"/>
         <v>0,59%</v>
       </c>
-      <c r="AB23" s="27" t="str">
-        <f>ROUND(P29,2)&amp;"%"</f>
+      <c r="AB23" s="26" t="str">
+        <f t="shared" si="1"/>
         <v>0,91%</v>
       </c>
     </row>
@@ -24207,20 +25232,20 @@
       <c r="X24" t="s">
         <v>623</v>
       </c>
-      <c r="Y24" s="27" t="str">
-        <f>ROUND(O13,2)&amp;"%"</f>
+      <c r="Y24" s="26" t="str">
+        <f t="shared" si="0"/>
         <v>3,39%</v>
       </c>
-      <c r="Z24" s="27" t="str">
-        <f>ROUND(P13,2)&amp;"%"</f>
+      <c r="Z24" s="26" t="str">
+        <f t="shared" si="0"/>
         <v>4,34%</v>
       </c>
-      <c r="AA24" s="27" t="str">
-        <f>ROUND(O30,2)&amp;"%"</f>
+      <c r="AA24" s="26" t="str">
+        <f t="shared" si="1"/>
         <v>0,81%</v>
       </c>
-      <c r="AB24" s="27" t="str">
-        <f>ROUND(P30,2)&amp;"%"</f>
+      <c r="AB24" s="26" t="str">
+        <f t="shared" si="1"/>
         <v>1,08%</v>
       </c>
     </row>
@@ -24249,20 +25274,20 @@
       <c r="X25" t="s">
         <v>624</v>
       </c>
-      <c r="Y25" s="27" t="str">
-        <f>ROUND(O14,2)&amp;"%"</f>
+      <c r="Y25" s="26" t="str">
+        <f t="shared" si="0"/>
         <v>3,33%</v>
       </c>
-      <c r="Z25" s="27" t="str">
-        <f>ROUND(P14,2)&amp;"%"</f>
+      <c r="Z25" s="26" t="str">
+        <f t="shared" si="0"/>
         <v>4,1%</v>
       </c>
-      <c r="AA25" s="27" t="str">
-        <f>ROUND(O31,2)&amp;"%"</f>
+      <c r="AA25" s="26" t="str">
+        <f t="shared" si="1"/>
         <v>0,73%</v>
       </c>
-      <c r="AB25" s="27" t="str">
-        <f>ROUND(P31,2)&amp;"%"</f>
+      <c r="AB25" s="26" t="str">
+        <f t="shared" si="1"/>
         <v>0,85%</v>
       </c>
     </row>
@@ -24425,23 +25450,23 @@
       <c r="AD29" t="s">
         <v>631</v>
       </c>
-      <c r="AE29" s="29">
+      <c r="AE29" s="27">
         <f>K11</f>
         <v>10.138339999999999</v>
       </c>
-      <c r="AF29" s="29">
+      <c r="AF29" s="27">
         <f>L11</f>
         <v>11.06123</v>
       </c>
-      <c r="AG29" s="29">
+      <c r="AG29" s="27">
         <f>K28</f>
         <v>6.7389569999999996E-2</v>
       </c>
-      <c r="AH29" s="29">
+      <c r="AH29" s="27">
         <f>L28</f>
         <v>9.6357360000000003E-2</v>
       </c>
-      <c r="AI29" s="29"/>
+      <c r="AI29" s="27"/>
     </row>
     <row r="30" spans="8:35" x14ac:dyDescent="0.35">
       <c r="H30" s="22"/>
@@ -24489,23 +25514,23 @@
       <c r="AD30" t="s">
         <v>622</v>
       </c>
-      <c r="AE30" s="29">
-        <f t="shared" ref="AE30:AF30" si="0">K12</f>
+      <c r="AE30" s="27">
+        <f t="shared" ref="AE30:AF30" si="2">K12</f>
         <v>5.3612840000000004</v>
       </c>
-      <c r="AF30" s="29">
-        <f t="shared" si="0"/>
+      <c r="AF30" s="27">
+        <f t="shared" si="2"/>
         <v>7.6462380000000003</v>
       </c>
-      <c r="AG30" s="29">
-        <f t="shared" ref="AG30:AG32" si="1">K29</f>
+      <c r="AG30" s="27">
+        <f t="shared" ref="AG30:AG32" si="3">K29</f>
         <v>3.5456799999999997E-2</v>
       </c>
-      <c r="AH30" s="29">
-        <f t="shared" ref="AH30:AH32" si="2">L29</f>
+      <c r="AH30" s="27">
+        <f t="shared" ref="AH30:AH32" si="4">L29</f>
         <v>5.7688940000000001E-2</v>
       </c>
-      <c r="AI30" s="29"/>
+      <c r="AI30" s="27"/>
     </row>
     <row r="31" spans="8:35" x14ac:dyDescent="0.35">
       <c r="I31" t="s">
@@ -24551,23 +25576,23 @@
       <c r="AD31" t="s">
         <v>623</v>
       </c>
-      <c r="AE31" s="29">
-        <f t="shared" ref="AE31:AF31" si="3">K13</f>
+      <c r="AE31" s="27">
+        <f t="shared" ref="AE31:AF31" si="5">K13</f>
         <v>5.9704059999999997</v>
       </c>
-      <c r="AF31" s="29">
+      <c r="AF31" s="27">
+        <f t="shared" si="5"/>
+        <v>7.6325320000000003</v>
+      </c>
+      <c r="AG31" s="27">
         <f t="shared" si="3"/>
-        <v>7.6325320000000003</v>
-      </c>
-      <c r="AG31" s="29">
-        <f t="shared" si="1"/>
         <v>4.9312519999999999E-2</v>
       </c>
-      <c r="AH31" s="29">
-        <f t="shared" si="2"/>
+      <c r="AH31" s="27">
+        <f t="shared" si="4"/>
         <v>6.2136660000000003E-2</v>
       </c>
-      <c r="AI31" s="29"/>
+      <c r="AI31" s="27"/>
     </row>
     <row r="32" spans="8:35" x14ac:dyDescent="0.35">
       <c r="I32" s="10" t="s">
@@ -24617,23 +25642,23 @@
       <c r="AD32" t="s">
         <v>624</v>
       </c>
-      <c r="AE32" s="29">
-        <f t="shared" ref="AE32:AF32" si="4">K14</f>
+      <c r="AE32" s="27">
+        <f t="shared" ref="AE32:AF32" si="6">K14</f>
         <v>7.4797289999999998</v>
       </c>
-      <c r="AF32" s="29">
+      <c r="AF32" s="27">
+        <f t="shared" si="6"/>
+        <v>7.5066800000000002</v>
+      </c>
+      <c r="AG32" s="27">
+        <f t="shared" si="3"/>
+        <v>4.8549160000000001E-2</v>
+      </c>
+      <c r="AH32" s="27">
         <f t="shared" si="4"/>
-        <v>7.5066800000000002</v>
-      </c>
-      <c r="AG32" s="29">
-        <f t="shared" si="1"/>
-        <v>4.8549160000000001E-2</v>
-      </c>
-      <c r="AH32" s="29">
-        <f t="shared" si="2"/>
         <v>5.3747389999999999E-2</v>
       </c>
-      <c r="AI32" s="29"/>
+      <c r="AI32" s="27"/>
     </row>
     <row r="33" spans="9:32" x14ac:dyDescent="0.35">
       <c r="I33" t="s">
@@ -24685,18 +25710,18 @@
       </c>
     </row>
     <row r="35" spans="9:32" x14ac:dyDescent="0.35">
-      <c r="Y35" s="28" t="s">
+      <c r="Y35" s="30" t="s">
         <v>626</v>
       </c>
-      <c r="Z35" s="28"/>
-      <c r="AA35" s="28"/>
-      <c r="AB35" s="28"/>
-      <c r="AC35" s="28" t="s">
+      <c r="Z35" s="30"/>
+      <c r="AA35" s="30"/>
+      <c r="AB35" s="30"/>
+      <c r="AC35" s="30" t="s">
         <v>627</v>
       </c>
-      <c r="AD35" s="28"/>
-      <c r="AE35" s="28"/>
-      <c r="AF35" s="28"/>
+      <c r="AD35" s="30"/>
+      <c r="AE35" s="30"/>
+      <c r="AF35" s="30"/>
     </row>
     <row r="36" spans="9:32" x14ac:dyDescent="0.35">
       <c r="I36" s="10" t="s">
@@ -24724,22 +25749,22 @@
       <c r="Q36" t="s">
         <v>600</v>
       </c>
-      <c r="Y36" s="28" t="s">
+      <c r="Y36" s="30" t="s">
         <v>628</v>
       </c>
-      <c r="Z36" s="28"/>
-      <c r="AA36" s="28" t="s">
+      <c r="Z36" s="30"/>
+      <c r="AA36" s="30" t="s">
         <v>629</v>
       </c>
-      <c r="AB36" s="28"/>
-      <c r="AC36" s="28" t="s">
+      <c r="AB36" s="30"/>
+      <c r="AC36" s="30" t="s">
         <v>628</v>
       </c>
-      <c r="AD36" s="28"/>
-      <c r="AE36" s="28" t="s">
+      <c r="AD36" s="30"/>
+      <c r="AE36" s="30" t="s">
         <v>630</v>
       </c>
-      <c r="AF36" s="28"/>
+      <c r="AF36" s="30"/>
     </row>
     <row r="37" spans="9:32" x14ac:dyDescent="0.35">
       <c r="I37" t="s">
@@ -24816,28 +25841,28 @@
       <c r="Y38" s="25">
         <v>1</v>
       </c>
-      <c r="Z38" s="27" t="str">
+      <c r="Z38" s="26" t="str">
         <f>ROUND(O11,2)&amp;"%"</f>
         <v>5,46%</v>
       </c>
       <c r="AA38" s="25">
         <v>1</v>
       </c>
-      <c r="AB38" s="27" t="str">
+      <c r="AB38" s="26" t="str">
         <f>ROUND(P11,2)&amp;"%"</f>
         <v>5,09%</v>
       </c>
       <c r="AC38" s="25">
         <v>1</v>
       </c>
-      <c r="AD38" s="27" t="str">
+      <c r="AD38" s="26" t="str">
         <f>ROUND(O28,2)&amp;"%"</f>
         <v>1,08%</v>
       </c>
       <c r="AE38" s="25">
         <v>1</v>
       </c>
-      <c r="AF38" s="27" t="str">
+      <c r="AF38" s="26" t="str">
         <f>ROUND(P28,2)&amp;"%"</f>
         <v>1,48%</v>
       </c>
@@ -24874,29 +25899,29 @@
       <c r="Y39" s="25">
         <v>0.52881280367397432</v>
       </c>
-      <c r="Z39" s="27" t="str">
-        <f t="shared" ref="Z39:Z41" si="5">ROUND(O12,2)&amp;"%"</f>
+      <c r="Z39" s="26" t="str">
+        <f t="shared" ref="Z39:Z41" si="7">ROUND(O12,2)&amp;"%"</f>
         <v>3,19%</v>
       </c>
       <c r="AA39" s="25">
         <v>0.69126471468362927</v>
       </c>
-      <c r="AB39" s="27" t="str">
-        <f t="shared" ref="AB39:AB41" si="6">ROUND(P12,2)&amp;"%"</f>
+      <c r="AB39" s="26" t="str">
+        <f t="shared" ref="AB39:AB41" si="8">ROUND(P12,2)&amp;"%"</f>
         <v>4,32%</v>
       </c>
       <c r="AC39" s="25">
         <v>0.5261467019302839</v>
       </c>
-      <c r="AD39" s="27" t="str">
-        <f t="shared" ref="AD39:AD41" si="7">ROUND(O29,2)&amp;"%"</f>
+      <c r="AD39" s="26" t="str">
+        <f t="shared" ref="AD39:AD41" si="9">ROUND(O29,2)&amp;"%"</f>
         <v>0,59%</v>
       </c>
       <c r="AE39" s="25">
         <v>0.59869780575142362</v>
       </c>
-      <c r="AF39" s="27" t="str">
-        <f t="shared" ref="AF39:AF41" si="8">ROUND(P29,2)&amp;"%"</f>
+      <c r="AF39" s="26" t="str">
+        <f t="shared" ref="AF39:AF41" si="10">ROUND(P29,2)&amp;"%"</f>
         <v>0,91%</v>
       </c>
     </row>
@@ -24928,29 +25953,29 @@
       <c r="Y40" s="25">
         <v>0.58889384258172439</v>
       </c>
-      <c r="Z40" s="27" t="str">
-        <f t="shared" si="5"/>
+      <c r="Z40" s="26" t="str">
+        <f t="shared" si="7"/>
         <v>3,39%</v>
       </c>
       <c r="AA40" s="25">
         <v>0.69002561197986123</v>
       </c>
-      <c r="AB40" s="27" t="str">
-        <f t="shared" si="6"/>
+      <c r="AB40" s="26" t="str">
+        <f t="shared" si="8"/>
         <v>4,34%</v>
       </c>
       <c r="AC40" s="25">
         <v>0.7317529997594584</v>
       </c>
-      <c r="AD40" s="27" t="str">
-        <f t="shared" si="7"/>
+      <c r="AD40" s="26" t="str">
+        <f t="shared" si="9"/>
         <v>0,81%</v>
       </c>
       <c r="AE40" s="25">
         <v>0.64485639706193698</v>
       </c>
-      <c r="AF40" s="27" t="str">
-        <f t="shared" si="8"/>
+      <c r="AF40" s="26" t="str">
+        <f t="shared" si="10"/>
         <v>1,08%</v>
       </c>
     </row>
@@ -24982,34 +26007,34 @@
       <c r="Y41" s="25">
         <v>0</v>
       </c>
-      <c r="Z41" s="27" t="str">
-        <f t="shared" si="5"/>
+      <c r="Z41" s="26" t="str">
+        <f t="shared" si="7"/>
         <v>3,33%</v>
       </c>
       <c r="AA41" s="25">
         <v>0</v>
       </c>
-      <c r="AB41" s="27" t="str">
-        <f t="shared" si="6"/>
+      <c r="AB41" s="26" t="str">
+        <f t="shared" si="8"/>
         <v>4,1%</v>
       </c>
       <c r="AC41" s="25">
         <v>0.72042543081963584</v>
       </c>
-      <c r="AD41" s="27" t="str">
-        <f t="shared" si="7"/>
+      <c r="AD41" s="26" t="str">
+        <f t="shared" si="9"/>
         <v>0,73%</v>
       </c>
       <c r="AE41" s="25">
         <v>0.55779226413010896</v>
       </c>
-      <c r="AF41" s="27" t="str">
-        <f t="shared" si="8"/>
+      <c r="AF41" s="26" t="str">
+        <f t="shared" si="10"/>
         <v>0,85%</v>
       </c>
     </row>
     <row r="45" spans="9:32" x14ac:dyDescent="0.35">
-      <c r="X45" s="30"/>
+      <c r="X45" s="28"/>
       <c r="Y45">
         <v>1</v>
       </c>
@@ -25018,7 +26043,7 @@
       </c>
     </row>
     <row r="46" spans="9:32" x14ac:dyDescent="0.35">
-      <c r="X46" s="30" t="s">
+      <c r="X46" s="28" t="s">
         <v>622</v>
       </c>
       <c r="Y46" t="s">
@@ -25029,7 +26054,7 @@
       </c>
     </row>
     <row r="47" spans="9:32" x14ac:dyDescent="0.35">
-      <c r="X47" s="30" t="s">
+      <c r="X47" s="28" t="s">
         <v>623</v>
       </c>
       <c r="Y47" t="s">
@@ -25040,7 +26065,7 @@
       </c>
     </row>
     <row r="48" spans="9:32" x14ac:dyDescent="0.35">
-      <c r="X48" s="31" t="s">
+      <c r="X48" s="29" t="s">
         <v>624</v>
       </c>
       <c r="Y48" t="s">
@@ -25048,6 +26073,48 @@
       </c>
       <c r="Z48" t="s">
         <v>641</v>
+      </c>
+    </row>
+    <row r="50" spans="24:26" x14ac:dyDescent="0.35">
+      <c r="X50" s="28"/>
+      <c r="Y50">
+        <v>1</v>
+      </c>
+      <c r="Z50">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="51" spans="24:26" x14ac:dyDescent="0.35">
+      <c r="X51" s="28" t="s">
+        <v>622</v>
+      </c>
+      <c r="Y51" t="s">
+        <v>642</v>
+      </c>
+      <c r="Z51" t="s">
+        <v>643</v>
+      </c>
+    </row>
+    <row r="52" spans="24:26" x14ac:dyDescent="0.35">
+      <c r="X52" s="28" t="s">
+        <v>623</v>
+      </c>
+      <c r="Y52" t="s">
+        <v>644</v>
+      </c>
+      <c r="Z52" t="s">
+        <v>645</v>
+      </c>
+    </row>
+    <row r="53" spans="24:26" x14ac:dyDescent="0.35">
+      <c r="X53" s="29" t="s">
+        <v>624</v>
+      </c>
+      <c r="Y53" t="s">
+        <v>646</v>
+      </c>
+      <c r="Z53" t="s">
+        <v>647</v>
       </c>
     </row>
   </sheetData>
@@ -25064,7 +26131,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{32EB6AD7-BBCF-41A4-A705-09A536484B28}">
   <dimension ref="A1:A39"/>
   <sheetViews>

</xml_diff>